<commit_message>
Made file names uniform
</commit_message>
<xml_diff>
--- a/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
+++ b/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\landfiredisturbance\specifications\2_MechAdd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LANDFIRE\landfiredisturbance-clone\specifications\2_MechAdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1065,15 +1065,6 @@
     <t>Time Step 3 (233) Rules</t>
   </si>
   <si>
-    <t>Low Severity Mech Add</t>
-  </si>
-  <si>
-    <t>Moderate Severity MechAdd</t>
-  </si>
-  <si>
-    <t>High Severity MechAdd</t>
-  </si>
-  <si>
     <t>* = 0.85</t>
   </si>
   <si>
@@ -1444,6 +1435,15 @@
   </si>
   <si>
     <t>* = 1/0.25</t>
+  </si>
+  <si>
+    <t>Low Severity Mech Add (21)</t>
+  </si>
+  <si>
+    <t>Moderate Severity MechAdd (22)</t>
+  </si>
+  <si>
+    <t>High Severity MechAdd (23)</t>
   </si>
 </sst>
 </file>
@@ -2540,8 +2540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K952"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,24 +2563,24 @@
     <row r="1" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1" s="24" t="s">
-        <v>272</v>
+        <v>396</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="26"/>
       <c r="F1" s="27" t="s">
-        <v>273</v>
+        <v>397</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="34"/>
       <c r="I1" s="27" t="s">
-        <v>274</v>
+        <v>398</v>
       </c>
       <c r="J1" s="25"/>
       <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>13</v>
@@ -2615,17 +2615,17 @@
         <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D3" s="30"/>
       <c r="F3" s="29" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>0</v>
@@ -2650,7 +2650,7 @@
         <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>10</v>
@@ -2667,7 +2667,7 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2675,14 +2675,14 @@
         <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D7" s="30"/>
       <c r="F7" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I7" s="29" t="s">
         <v>1</v>
@@ -2693,14 +2693,14 @@
         <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D8" s="30"/>
       <c r="F8" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I8" s="29" t="s">
         <v>1</v>
@@ -2711,7 +2711,7 @@
         <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>0</v>
@@ -2728,7 +2728,7 @@
         <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>10</v>
@@ -2745,7 +2745,7 @@
         <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2753,14 +2753,14 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D12" s="30"/>
       <c r="F12" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I12" s="29" t="s">
         <v>1</v>
@@ -2771,14 +2771,14 @@
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D13" s="30"/>
       <c r="F13" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>1</v>
@@ -2789,7 +2789,7 @@
         <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>251</v>
@@ -2803,7 +2803,7 @@
         <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>251</v>
@@ -2817,7 +2817,7 @@
         <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>251</v>
@@ -2831,7 +2831,7 @@
         <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>1</v>
@@ -2848,7 +2848,7 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>1</v>
@@ -2865,7 +2865,7 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2873,7 +2873,7 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
         <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2889,7 +2889,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E22" s="31"/>
     </row>
@@ -2898,7 +2898,7 @@
         <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="31"/>
@@ -2910,7 +2910,7 @@
         <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E24" s="31"/>
       <c r="G24" s="30"/>
@@ -2921,7 +2921,7 @@
         <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="31"/>
@@ -2931,7 +2931,7 @@
         <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E26" s="31"/>
     </row>
@@ -2940,7 +2940,7 @@
         <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2972,7 +2972,7 @@
         <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2988,7 +2988,7 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E35" s="31"/>
       <c r="J35" s="30"/>
@@ -3015,10 +3015,10 @@
         <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>0</v>
@@ -3027,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>10</v>
@@ -3050,27 +3050,27 @@
         <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="29" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H37" s="31"/>
       <c r="I37" s="29" t="s">
         <v>1</v>
       </c>
       <c r="J37" s="30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K37" s="31"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E38" s="31"/>
       <c r="H38" s="31"/>
@@ -3090,10 +3090,10 @@
         <v>140</v>
       </c>
       <c r="B39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>0</v>
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G39" s="30" t="s">
         <v>10</v>
@@ -3125,20 +3125,20 @@
         <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="29" t="s">
         <v>1</v>
       </c>
       <c r="G40" s="30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H40" s="31"/>
       <c r="I40" s="29" t="s">
@@ -3154,7 +3154,7 @@
         <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D41" s="30"/>
       <c r="G41" s="30"/>
@@ -3166,19 +3166,19 @@
         <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>12</v>
@@ -3201,19 +3201,19 @@
         <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D43" s="30" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>12</v>
@@ -3236,26 +3236,26 @@
         <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G44" s="30" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I44" s="29" t="s">
         <v>1</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="K44" s="31"/>
     </row>
@@ -3264,7 +3264,7 @@
         <v>118</v>
       </c>
       <c r="B45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D45" s="30"/>
       <c r="J45" s="30"/>
@@ -3275,16 +3275,16 @@
         <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>10</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>12</v>
@@ -3307,16 +3307,16 @@
         <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D47" s="30" t="s">
         <v>10</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>12</v>
@@ -3339,25 +3339,25 @@
         <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G48" s="30" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I48" s="29" t="s">
         <v>1</v>
       </c>
       <c r="J48" s="30" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="K48" s="31"/>
     </row>
@@ -3366,34 +3366,34 @@
         <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C49" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F49" s="29" t="s">
         <v>12</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I49" s="29" t="s">
         <v>263</v>
       </c>
       <c r="J49" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3401,34 +3401,34 @@
         <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F50" s="29" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I50" s="29" t="s">
         <v>263</v>
       </c>
       <c r="J50" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,34 +3436,34 @@
         <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C51" s="29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H51" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3471,34 +3471,34 @@
         <v>148</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F52" s="29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G52" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H52" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I52" s="29" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J52" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K52" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3506,34 +3506,34 @@
         <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F53" s="29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H53" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I53" s="29" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J53" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K53" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
         <v>209</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D54" s="33">
         <v>0.75</v>
@@ -3559,7 +3559,7 @@
         <v>210</v>
       </c>
       <c r="B55" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D55" s="33">
         <v>0.75</v>
@@ -3577,7 +3577,7 @@
         <v>211</v>
       </c>
       <c r="B56" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D56" s="33">
         <v>0.75</v>
@@ -3595,25 +3595,25 @@
         <v>212</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D57" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="E57" s="31" t="s">
         <v>383</v>
       </c>
-      <c r="E57" s="31" t="s">
-        <v>386</v>
-      </c>
       <c r="G57" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="H57" s="31" t="s">
         <v>383</v>
       </c>
-      <c r="H57" s="31" t="s">
-        <v>386</v>
-      </c>
       <c r="J57" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="K57" s="31" t="s">
         <v>383</v>
-      </c>
-      <c r="K57" s="31" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3621,25 +3621,25 @@
         <v>213</v>
       </c>
       <c r="B58" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D58" s="42" t="s">
+        <v>381</v>
+      </c>
+      <c r="E58" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="E58" s="31" t="s">
-        <v>387</v>
-      </c>
       <c r="G58" s="42" t="s">
+        <v>381</v>
+      </c>
+      <c r="H58" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="H58" s="31" t="s">
-        <v>387</v>
-      </c>
       <c r="J58" s="42" t="s">
+        <v>381</v>
+      </c>
+      <c r="K58" s="31" t="s">
         <v>384</v>
-      </c>
-      <c r="K58" s="31" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3647,25 +3647,25 @@
         <v>214</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D59" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="E59" s="31" t="s">
         <v>385</v>
       </c>
-      <c r="E59" s="31" t="s">
-        <v>388</v>
-      </c>
       <c r="G59" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="H59" s="31" t="s">
         <v>385</v>
       </c>
-      <c r="H59" s="31" t="s">
-        <v>388</v>
-      </c>
       <c r="J59" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="K59" s="31" t="s">
         <v>385</v>
-      </c>
-      <c r="K59" s="31" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3673,7 +3673,7 @@
         <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3689,25 +3689,25 @@
         <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H62" s="31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I62" s="29" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K62" s="31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
         <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
         <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3731,16 +3731,16 @@
         <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H65" s="31" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K65" s="31" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -3748,7 +3748,7 @@
         <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -3756,7 +3756,7 @@
         <v>151</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
         <v>152</v>
       </c>
       <c r="B68" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3780,7 +3780,7 @@
         <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3788,7 +3788,7 @@
         <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
         <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3804,7 +3804,7 @@
         <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3812,7 +3812,7 @@
         <v>124</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3820,7 +3820,7 @@
         <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>126</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -3836,7 +3836,7 @@
         <v>127</v>
       </c>
       <c r="B77" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -3844,7 +3844,7 @@
         <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -3852,7 +3852,7 @@
         <v>129</v>
       </c>
       <c r="B79" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D79" s="30"/>
       <c r="J79" s="30"/>
@@ -3862,7 +3862,7 @@
         <v>130</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D80" s="30"/>
       <c r="J80" s="30"/>
@@ -3872,7 +3872,7 @@
         <v>131</v>
       </c>
       <c r="B81" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C81" s="29" t="s">
         <v>10</v>
@@ -3893,7 +3893,7 @@
         <v>132</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C82" s="29" t="s">
         <v>10</v>
@@ -3914,7 +3914,7 @@
         <v>133</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D83" s="30"/>
       <c r="J83" s="30"/>
@@ -3924,7 +3924,7 @@
         <v>134</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D84" s="30"/>
       <c r="J84" s="30"/>
@@ -3934,7 +3934,7 @@
         <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D85" s="30"/>
     </row>
@@ -3943,7 +3943,7 @@
         <v>108</v>
       </c>
       <c r="B86" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D86" s="30"/>
     </row>
@@ -3952,7 +3952,7 @@
         <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D87" s="30"/>
       <c r="E87" s="31"/>
@@ -3968,7 +3968,7 @@
         <v>110</v>
       </c>
       <c r="B88" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D88" s="30"/>
       <c r="H88" s="31" t="s">
@@ -3983,7 +3983,7 @@
         <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D89" s="30"/>
     </row>
@@ -3992,7 +3992,7 @@
         <v>105</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D90" s="30"/>
     </row>
@@ -4001,7 +4001,7 @@
         <v>106</v>
       </c>
       <c r="B91" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D91" s="30"/>
     </row>
@@ -4010,7 +4010,7 @@
         <v>111</v>
       </c>
       <c r="B92" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D92" s="30"/>
     </row>
@@ -4019,7 +4019,7 @@
         <v>112</v>
       </c>
       <c r="B93" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D93" s="30"/>
     </row>
@@ -4028,7 +4028,7 @@
         <v>113</v>
       </c>
       <c r="B94" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D94" s="30"/>
     </row>
@@ -7406,7 +7406,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>264</v>
@@ -7494,7 +7494,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C3" s="5">
         <v>0.85</v>
@@ -7592,7 +7592,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" s="5">
         <v>1.1000000000000001</v>
@@ -7690,7 +7690,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" s="5">
         <v>1.25</v>
@@ -7788,7 +7788,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
@@ -7884,7 +7884,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C7" s="5">
         <v>0.75</v>
@@ -7982,7 +7982,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C8" s="5">
         <v>0.75</v>
@@ -8080,7 +8080,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C9" s="5">
         <v>1.25</v>
@@ -8169,7 +8169,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C10" s="5">
         <v>1.25</v>
@@ -8258,7 +8258,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -8345,7 +8345,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" s="5">
         <v>0.75</v>
@@ -8434,7 +8434,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C13" s="5">
         <v>0.75</v>
@@ -8523,7 +8523,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -8616,7 +8616,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -8709,7 +8709,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -8802,7 +8802,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C17" s="5">
         <v>0.25</v>
@@ -8897,7 +8897,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C18" s="5">
         <v>0.25</v>
@@ -8992,7 +8992,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -9082,7 +9082,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -9172,7 +9172,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -9262,7 +9262,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -9349,7 +9349,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -9436,7 +9436,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -9523,7 +9523,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -9610,7 +9610,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -9697,7 +9697,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -9790,7 +9790,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -9883,7 +9883,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -9976,7 +9976,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
@@ -10072,7 +10072,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
@@ -10168,7 +10168,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -10264,7 +10264,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -10354,7 +10354,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -10444,7 +10444,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -10546,7 +10546,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C36" s="5">
         <v>0.75</v>
@@ -10654,7 +10654,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B37" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C37" s="5">
         <v>0.5</v>
@@ -10762,7 +10762,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B38" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -10855,7 +10855,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C39" s="5">
         <v>0.75</v>
@@ -10954,7 +10954,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B40" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C40" s="5">
         <v>0.5</v>
@@ -11053,7 +11053,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -11152,7 +11152,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C42" s="5">
         <v>0.75</v>
@@ -11257,7 +11257,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B43" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C43" s="5">
         <v>0.75</v>
@@ -11362,7 +11362,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B44" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C44" s="5">
         <v>0.75</v>
@@ -11465,7 +11465,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
@@ -11561,7 +11561,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C46" s="5">
         <v>0.75</v>
@@ -11661,7 +11661,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C47" s="5">
         <v>0.75</v>
@@ -11761,7 +11761,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C48" s="5">
         <v>0.75</v>
@@ -11861,7 +11861,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C49" s="5">
         <v>1.25</v>
@@ -11966,7 +11966,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" s="5">
         <v>1.25</v>
@@ -12071,7 +12071,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B51" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C51" s="5">
         <v>1.25</v>
@@ -12176,7 +12176,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C52" s="5">
         <v>1.25</v>
@@ -12281,7 +12281,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C53" s="5">
         <v>1.25</v>
@@ -12386,7 +12386,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6">
@@ -12489,7 +12489,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6">
@@ -12592,7 +12592,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="6">
@@ -12695,7 +12695,7 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="6">
@@ -12792,7 +12792,7 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6">
@@ -12889,7 +12889,7 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="6">
@@ -12986,7 +12986,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
@@ -13078,7 +13078,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B61" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
@@ -13170,7 +13170,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C62" s="5">
         <v>0.25</v>
@@ -13264,7 +13264,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B63" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
@@ -13360,7 +13360,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
@@ -13456,12 +13456,12 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
       <c r="E65" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F65" s="13">
         <v>115</v>
@@ -13554,7 +13554,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B66" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
@@ -13638,7 +13638,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
@@ -13722,7 +13722,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B68" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
@@ -13806,7 +13806,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -13908,7 +13908,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
@@ -14010,7 +14010,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B71" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
@@ -14112,7 +14112,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
@@ -14199,7 +14199,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -14286,7 +14286,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
@@ -14373,7 +14373,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
@@ -14466,7 +14466,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -14556,7 +14556,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
@@ -14643,7 +14643,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B78" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
@@ -14727,7 +14727,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B79" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="6"/>
@@ -14814,7 +14814,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="6"/>
@@ -14901,7 +14901,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B81" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C81" s="5">
         <v>1.25</v>
@@ -15005,7 +15005,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C82" s="5">
         <v>1.25</v>
@@ -15109,7 +15109,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
@@ -15199,7 +15199,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
@@ -15289,7 +15289,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B85" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
@@ -15379,7 +15379,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B86" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
@@ -15469,7 +15469,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B87" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
@@ -15571,7 +15571,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B88" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
@@ -15673,7 +15673,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -15757,7 +15757,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -15841,7 +15841,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B91" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
@@ -15925,7 +15925,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B92" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
@@ -16012,7 +16012,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B93" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
@@ -16099,7 +16099,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B94" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>
@@ -16247,7 +16247,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>266</v>
@@ -16337,7 +16337,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C3" s="5">
         <v>0.67</v>
@@ -16435,7 +16435,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" s="5">
         <v>1.25</v>
@@ -16533,7 +16533,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" s="5">
         <v>1.5</v>
@@ -16631,7 +16631,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="9"/>
@@ -16652,7 +16652,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="14">
-        <f t="shared" ref="K6:K21" si="7">J6</f>
+        <f t="shared" ref="K6" si="7">J6</f>
         <v>0</v>
       </c>
       <c r="L6" s="18">
@@ -16664,7 +16664,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="14">
-        <f t="shared" ref="O6:O21" si="9">N6</f>
+        <f t="shared" ref="O6" si="9">N6</f>
         <v>0</v>
       </c>
       <c r="P6" s="18">
@@ -16679,7 +16679,7 @@
         <v>25</v>
       </c>
       <c r="S6" s="14">
-        <f t="shared" ref="S6:S21" si="11">R6</f>
+        <f t="shared" ref="S6" si="11">R6</f>
         <v>25</v>
       </c>
       <c r="T6" s="18">
@@ -16694,7 +16694,7 @@
         <v>60</v>
       </c>
       <c r="W6" s="14">
-        <f t="shared" ref="W6:W21" si="13">V6</f>
+        <f t="shared" ref="W6" si="13">V6</f>
         <v>60</v>
       </c>
       <c r="X6" s="18">
@@ -16709,7 +16709,7 @@
         <v>78</v>
       </c>
       <c r="AA6" s="14">
-        <f t="shared" ref="AA6:AA21" si="15">Z6</f>
+        <f t="shared" ref="AA6" si="15">Z6</f>
         <v>78</v>
       </c>
       <c r="AB6" s="18">
@@ -16727,7 +16727,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C7" s="5">
         <v>0.5</v>
@@ -16825,7 +16825,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C8" s="5">
         <v>0.5</v>
@@ -16923,7 +16923,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C9" s="5">
         <v>1.25</v>
@@ -17012,7 +17012,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C10" s="5">
         <v>1.5</v>
@@ -17101,7 +17101,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="9"/>
@@ -17119,7 +17119,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="14">
-        <f t="shared" ref="K11:K26" si="17">J11</f>
+        <f t="shared" ref="K11" si="17">J11</f>
         <v>0</v>
       </c>
       <c r="L11" s="18">
@@ -17131,7 +17131,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="14">
-        <f t="shared" ref="O11:O26" si="18">N11</f>
+        <f t="shared" ref="O11" si="18">N11</f>
         <v>0</v>
       </c>
       <c r="P11" s="18">
@@ -17143,7 +17143,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="14">
-        <f t="shared" ref="S11:S26" si="19">R11</f>
+        <f t="shared" ref="S11" si="19">R11</f>
         <v>0</v>
       </c>
       <c r="T11" s="18">
@@ -17158,7 +17158,7 @@
         <v>44</v>
       </c>
       <c r="W11" s="14">
-        <f t="shared" ref="W11:W26" si="20">V11</f>
+        <f t="shared" ref="W11" si="20">V11</f>
         <v>44</v>
       </c>
       <c r="X11" s="18">
@@ -17170,7 +17170,7 @@
         <v>44</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" ref="AA11:AA26" si="21">Z11</f>
+        <f t="shared" ref="AA11" si="21">Z11</f>
         <v>0</v>
       </c>
       <c r="AB11" s="18">
@@ -17188,7 +17188,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" s="5">
         <v>0.5</v>
@@ -17277,7 +17277,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C13" s="5">
         <v>0.5</v>
@@ -17366,7 +17366,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
@@ -17461,7 +17461,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C15" s="5">
         <v>0</v>
@@ -17556,7 +17556,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -17651,7 +17651,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C17" s="5">
         <v>0</v>
@@ -17746,7 +17746,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -17841,7 +17841,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9"/>
@@ -17931,7 +17931,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="9"/>
@@ -18021,7 +18021,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="9"/>
@@ -18111,7 +18111,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="9"/>
@@ -18198,7 +18198,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
@@ -18285,7 +18285,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="9"/>
@@ -18372,7 +18372,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="9"/>
@@ -18459,7 +18459,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="9"/>
@@ -18546,7 +18546,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9"/>
@@ -18639,7 +18639,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="9"/>
@@ -18732,7 +18732,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="9"/>
@@ -18825,7 +18825,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="9"/>
@@ -18921,7 +18921,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="9"/>
@@ -19017,7 +19017,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9"/>
@@ -19113,7 +19113,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9"/>
@@ -19203,7 +19203,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9"/>
@@ -19293,7 +19293,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9"/>
@@ -19325,7 +19325,7 @@
         <v>5</v>
       </c>
       <c r="M35" s="19">
-        <f t="shared" ref="M35:M48" si="41">L35</f>
+        <f t="shared" ref="M35" si="41">L35</f>
         <v>5</v>
       </c>
       <c r="N35" s="13">
@@ -19340,7 +19340,7 @@
         <v>3</v>
       </c>
       <c r="Q35" s="19">
-        <f t="shared" ref="Q35:Q48" si="42">P35</f>
+        <f t="shared" ref="Q35" si="42">P35</f>
         <v>3</v>
       </c>
       <c r="R35" s="13">
@@ -19355,7 +19355,7 @@
         <v>5</v>
       </c>
       <c r="U35" s="19">
-        <f t="shared" ref="U35:U48" si="43">T35</f>
+        <f t="shared" ref="U35" si="43">T35</f>
         <v>5</v>
       </c>
       <c r="V35" s="13">
@@ -19370,7 +19370,7 @@
         <v>6</v>
       </c>
       <c r="Y35" s="19">
-        <f t="shared" ref="Y35:Y48" si="44">X35</f>
+        <f t="shared" ref="Y35" si="44">X35</f>
         <v>6</v>
       </c>
       <c r="Z35" s="13">
@@ -19385,7 +19385,7 @@
         <v>5</v>
       </c>
       <c r="AC35" s="19">
-        <f t="shared" ref="AC35:AC48" si="45">AB35</f>
+        <f t="shared" ref="AC35" si="45">AB35</f>
         <v>5</v>
       </c>
     </row>
@@ -19395,7 +19395,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C36" s="5">
         <v>0.5</v>
@@ -19503,7 +19503,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B37" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C37" s="5">
         <v>0.25</v>
@@ -19609,7 +19609,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B38" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9"/>
@@ -19633,66 +19633,66 @@
         <v>2</v>
       </c>
       <c r="K38" s="14">
-        <f t="shared" ref="K38:K45" si="47">J38</f>
+        <f t="shared" ref="K38" si="47">J38</f>
         <v>2</v>
       </c>
       <c r="L38" s="18">
-        <f t="shared" ref="L38:L45" si="48">K38</f>
+        <f t="shared" ref="L38" si="48">K38</f>
         <v>2</v>
       </c>
       <c r="M38" s="19">
-        <f t="shared" ref="M38:M51" si="49">L38</f>
+        <f t="shared" ref="M38" si="49">L38</f>
         <v>2</v>
       </c>
       <c r="O38" s="14">
-        <f t="shared" ref="O38:O45" si="50">N38</f>
+        <f t="shared" ref="O38" si="50">N38</f>
         <v>0</v>
       </c>
       <c r="P38" s="18">
-        <f t="shared" ref="P38:P45" si="51">O38</f>
+        <f t="shared" ref="P38" si="51">O38</f>
         <v>0</v>
       </c>
       <c r="Q38" s="19">
-        <f t="shared" ref="Q38:Q51" si="52">P38</f>
+        <f t="shared" ref="Q38" si="52">P38</f>
         <v>0</v>
       </c>
       <c r="R38" s="13">
         <v>1</v>
       </c>
       <c r="S38" s="14">
-        <f t="shared" ref="S38:S45" si="53">R38</f>
+        <f t="shared" ref="S38" si="53">R38</f>
         <v>1</v>
       </c>
       <c r="T38" s="18">
-        <f t="shared" ref="T38:T45" si="54">S38</f>
+        <f t="shared" ref="T38" si="54">S38</f>
         <v>1</v>
       </c>
       <c r="U38" s="19">
-        <f t="shared" ref="U38:U51" si="55">T38</f>
+        <f t="shared" ref="U38" si="55">T38</f>
         <v>1</v>
       </c>
       <c r="W38" s="14">
-        <f t="shared" ref="W38:W45" si="56">V38</f>
+        <f t="shared" ref="W38" si="56">V38</f>
         <v>0</v>
       </c>
       <c r="X38" s="18">
-        <f t="shared" ref="X38:X45" si="57">W38</f>
+        <f t="shared" ref="X38" si="57">W38</f>
         <v>0</v>
       </c>
       <c r="Y38" s="19">
-        <f t="shared" ref="Y38:Y51" si="58">X38</f>
+        <f t="shared" ref="Y38" si="58">X38</f>
         <v>0</v>
       </c>
       <c r="AA38" s="14">
-        <f t="shared" ref="AA38:AA45" si="59">Z38</f>
+        <f t="shared" ref="AA38" si="59">Z38</f>
         <v>0</v>
       </c>
       <c r="AB38" s="18">
-        <f t="shared" ref="AB38:AB45" si="60">AA38</f>
+        <f t="shared" ref="AB38" si="60">AA38</f>
         <v>0</v>
       </c>
       <c r="AC38" s="19">
-        <f t="shared" ref="AC38:AC51" si="61">AB38</f>
+        <f t="shared" ref="AC38" si="61">AB38</f>
         <v>0</v>
       </c>
     </row>
@@ -19702,7 +19702,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C39" s="5">
         <v>0.5</v>
@@ -19801,7 +19801,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B40" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C40" s="5">
         <v>0.25</v>
@@ -19898,7 +19898,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9"/>
@@ -19919,75 +19919,75 @@
         <v>0.9</v>
       </c>
       <c r="K41" s="14">
-        <f t="shared" ref="K41:K48" si="62">J41</f>
+        <f t="shared" ref="K41" si="62">J41</f>
         <v>0</v>
       </c>
       <c r="L41" s="18">
-        <f t="shared" ref="L41:L48" si="63">K41</f>
+        <f t="shared" ref="L41" si="63">K41</f>
         <v>0</v>
       </c>
       <c r="M41" s="19">
-        <f t="shared" ref="M41:M54" si="64">L41</f>
+        <f t="shared" ref="M41" si="64">L41</f>
         <v>0</v>
       </c>
       <c r="N41" s="13">
         <v>2</v>
       </c>
       <c r="O41" s="14">
-        <f t="shared" ref="O41:O48" si="65">N41</f>
+        <f t="shared" ref="O41" si="65">N41</f>
         <v>2</v>
       </c>
       <c r="P41" s="18">
-        <f t="shared" ref="P41:P48" si="66">O41</f>
+        <f t="shared" ref="P41" si="66">O41</f>
         <v>2</v>
       </c>
       <c r="Q41" s="19">
-        <f t="shared" ref="Q41:Q54" si="67">P41</f>
+        <f t="shared" ref="Q41" si="67">P41</f>
         <v>2</v>
       </c>
       <c r="R41" s="13">
         <v>1</v>
       </c>
       <c r="S41" s="14">
-        <f t="shared" ref="S41:S48" si="68">R41</f>
+        <f t="shared" ref="S41" si="68">R41</f>
         <v>1</v>
       </c>
       <c r="T41" s="18">
-        <f t="shared" ref="T41:T48" si="69">S41</f>
+        <f t="shared" ref="T41" si="69">S41</f>
         <v>1</v>
       </c>
       <c r="U41" s="19">
-        <f t="shared" ref="U41:U54" si="70">T41</f>
+        <f t="shared" ref="U41" si="70">T41</f>
         <v>1</v>
       </c>
       <c r="V41" s="13">
         <v>2.5</v>
       </c>
       <c r="W41" s="14">
-        <f t="shared" ref="W41:W48" si="71">V41</f>
+        <f t="shared" ref="W41" si="71">V41</f>
         <v>2.5</v>
       </c>
       <c r="X41" s="18">
-        <f t="shared" ref="X41:X48" si="72">W41</f>
+        <f t="shared" ref="X41" si="72">W41</f>
         <v>2.5</v>
       </c>
       <c r="Y41" s="19">
-        <f t="shared" ref="Y41:Y54" si="73">X41</f>
+        <f t="shared" ref="Y41" si="73">X41</f>
         <v>2.5</v>
       </c>
       <c r="Z41" s="13">
         <v>2</v>
       </c>
       <c r="AA41" s="14">
-        <f t="shared" ref="AA41:AA48" si="74">Z41</f>
+        <f t="shared" ref="AA41" si="74">Z41</f>
         <v>2</v>
       </c>
       <c r="AB41" s="18">
-        <f t="shared" ref="AB41:AB48" si="75">AA41</f>
+        <f t="shared" ref="AB41" si="75">AA41</f>
         <v>2</v>
       </c>
       <c r="AC41" s="19">
-        <f t="shared" ref="AC41:AC54" si="76">AB41</f>
+        <f t="shared" ref="AC41" si="76">AB41</f>
         <v>2</v>
       </c>
     </row>
@@ -19997,7 +19997,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C42" s="5">
         <v>0.5</v>
@@ -20102,7 +20102,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B43" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C43" s="5">
         <v>0.5</v>
@@ -20207,7 +20207,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B44" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C44" s="5">
         <v>0.5</v>
@@ -20240,7 +20240,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="19">
-        <f t="shared" ref="M44:M57" si="77">L44</f>
+        <f t="shared" ref="M44:M45" si="77">L44</f>
         <v>0</v>
       </c>
       <c r="N44" s="13">
@@ -20255,7 +20255,7 @@
         <v>63.75</v>
       </c>
       <c r="Q44" s="19">
-        <f t="shared" ref="Q44:Q57" si="78">P44</f>
+        <f t="shared" ref="Q44:Q45" si="78">P44</f>
         <v>63.75</v>
       </c>
       <c r="R44" s="13">
@@ -20270,7 +20270,7 @@
         <v>67.5</v>
       </c>
       <c r="U44" s="19">
-        <f t="shared" ref="U44:U57" si="79">T44</f>
+        <f t="shared" ref="U44:U45" si="79">T44</f>
         <v>67.5</v>
       </c>
       <c r="V44" s="13">
@@ -20285,7 +20285,7 @@
         <v>60</v>
       </c>
       <c r="Y44" s="19">
-        <f t="shared" ref="Y44:Y57" si="80">X44</f>
+        <f t="shared" ref="Y44:Y45" si="80">X44</f>
         <v>60</v>
       </c>
       <c r="Z44" s="13">
@@ -20300,7 +20300,7 @@
         <v>45</v>
       </c>
       <c r="AC44" s="19">
-        <f t="shared" ref="AC44:AC57" si="81">AB44</f>
+        <f t="shared" ref="AC44:AC45" si="81">AB44</f>
         <v>45</v>
       </c>
     </row>
@@ -20310,7 +20310,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="9"/>
@@ -20331,11 +20331,11 @@
         <v>0.9</v>
       </c>
       <c r="K45" s="14">
-        <f t="shared" ref="K45:K52" si="82">J45</f>
+        <f t="shared" ref="K45" si="82">J45</f>
         <v>0</v>
       </c>
       <c r="L45" s="18">
-        <f t="shared" ref="L45:L52" si="83">K45</f>
+        <f t="shared" ref="L45" si="83">K45</f>
         <v>0</v>
       </c>
       <c r="M45" s="19">
@@ -20346,11 +20346,11 @@
         <v>1</v>
       </c>
       <c r="O45" s="14">
-        <f t="shared" ref="O45:O52" si="84">N45</f>
+        <f t="shared" ref="O45" si="84">N45</f>
         <v>1</v>
       </c>
       <c r="P45" s="18">
-        <f t="shared" ref="P45:P52" si="85">O45</f>
+        <f t="shared" ref="P45" si="85">O45</f>
         <v>1</v>
       </c>
       <c r="Q45" s="19">
@@ -20361,11 +20361,11 @@
         <v>0.5</v>
       </c>
       <c r="S45" s="14">
-        <f t="shared" ref="S45:S52" si="86">R45</f>
+        <f t="shared" ref="S45" si="86">R45</f>
         <v>0.5</v>
       </c>
       <c r="T45" s="18">
-        <f t="shared" ref="T45:T52" si="87">S45</f>
+        <f t="shared" ref="T45" si="87">S45</f>
         <v>0.5</v>
       </c>
       <c r="U45" s="19">
@@ -20373,11 +20373,11 @@
         <v>0.5</v>
       </c>
       <c r="W45" s="14">
-        <f t="shared" ref="W45:W52" si="88">V45</f>
+        <f t="shared" ref="W45" si="88">V45</f>
         <v>0</v>
       </c>
       <c r="X45" s="18">
-        <f t="shared" ref="X45:X52" si="89">W45</f>
+        <f t="shared" ref="X45" si="89">W45</f>
         <v>0</v>
       </c>
       <c r="Y45" s="19">
@@ -20388,11 +20388,11 @@
         <v>1</v>
       </c>
       <c r="AA45" s="14">
-        <f t="shared" ref="AA45:AA52" si="90">Z45</f>
+        <f t="shared" ref="AA45" si="90">Z45</f>
         <v>1</v>
       </c>
       <c r="AB45" s="18">
-        <f t="shared" ref="AB45:AB52" si="91">AA45</f>
+        <f t="shared" ref="AB45" si="91">AA45</f>
         <v>1</v>
       </c>
       <c r="AC45" s="19">
@@ -20406,7 +20406,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C46" s="5">
         <v>0.75</v>
@@ -20508,7 +20508,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C47" s="5">
         <v>0.75</v>
@@ -20610,7 +20610,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C48" s="5">
         <v>0.75</v>
@@ -20643,7 +20643,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="19">
-        <f t="shared" ref="M48:M61" si="98">L48</f>
+        <f t="shared" ref="M48" si="98">L48</f>
         <v>0</v>
       </c>
       <c r="N48" s="13">
@@ -20658,7 +20658,7 @@
         <v>78.75</v>
       </c>
       <c r="Q48" s="19">
-        <f t="shared" ref="Q48:Q61" si="99">P48</f>
+        <f t="shared" ref="Q48" si="99">P48</f>
         <v>78.75</v>
       </c>
       <c r="R48" s="13">
@@ -20673,7 +20673,7 @@
         <v>101.25</v>
       </c>
       <c r="U48" s="19">
-        <f t="shared" ref="U48:U61" si="100">T48</f>
+        <f t="shared" ref="U48" si="100">T48</f>
         <v>101.25</v>
       </c>
       <c r="W48" s="14">
@@ -20685,7 +20685,7 @@
         <v>0</v>
       </c>
       <c r="Y48" s="19">
-        <f t="shared" ref="Y48:Y61" si="101">X48</f>
+        <f t="shared" ref="Y48" si="101">X48</f>
         <v>0</v>
       </c>
       <c r="Z48" s="13">
@@ -20700,7 +20700,7 @@
         <v>67.5</v>
       </c>
       <c r="AC48" s="19">
-        <f t="shared" ref="AC48:AC61" si="102">AB48</f>
+        <f t="shared" ref="AC48" si="102">AB48</f>
         <v>67.5</v>
       </c>
     </row>
@@ -20710,7 +20710,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C49" s="5">
         <v>1.5</v>
@@ -20815,7 +20815,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" s="5">
         <v>1.5</v>
@@ -20920,7 +20920,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B51" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C51" s="5">
         <v>1.5</v>
@@ -21025,7 +21025,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C52" s="5">
         <v>1.5</v>
@@ -21130,7 +21130,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C53" s="5">
         <v>1.5</v>
@@ -21235,7 +21235,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="9">
@@ -21261,7 +21261,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="14">
-        <f t="shared" ref="K54:K94" si="104">J54</f>
+        <f t="shared" ref="K54:K61" si="104">J54</f>
         <v>0</v>
       </c>
       <c r="L54" s="18">
@@ -21273,7 +21273,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="14">
-        <f t="shared" ref="O54:O94" si="105">N54</f>
+        <f t="shared" ref="O54:O61" si="105">N54</f>
         <v>0</v>
       </c>
       <c r="P54" s="18">
@@ -21288,7 +21288,7 @@
         <v>1</v>
       </c>
       <c r="S54" s="14">
-        <f t="shared" ref="S54:S94" si="106">R54</f>
+        <f t="shared" ref="S54:S61" si="106">R54</f>
         <v>1</v>
       </c>
       <c r="T54" s="18">
@@ -21303,7 +21303,7 @@
         <v>1.2</v>
       </c>
       <c r="W54" s="14">
-        <f t="shared" ref="W54:W94" si="107">V54</f>
+        <f t="shared" ref="W54:W61" si="107">V54</f>
         <v>1.2</v>
       </c>
       <c r="X54" s="18">
@@ -21318,7 +21318,7 @@
         <v>0.5</v>
       </c>
       <c r="AA54" s="14">
-        <f t="shared" ref="AA54:AA94" si="108">Z54</f>
+        <f t="shared" ref="AA54:AA61" si="108">Z54</f>
         <v>0.5</v>
       </c>
       <c r="AB54" s="18">
@@ -21336,7 +21336,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="9">
@@ -21437,7 +21437,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="9">
@@ -21538,14 +21538,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F57" s="13">
         <v>5</v>
@@ -21635,14 +21635,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F58" s="13">
         <v>11</v>
@@ -21732,14 +21732,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F59" s="13">
         <v>0</v>
@@ -21829,7 +21829,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="9"/>
@@ -21854,7 +21854,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="18">
-        <f t="shared" ref="L60:M100" si="109">K60</f>
+        <f t="shared" ref="L60:M94" si="109">K60</f>
         <v>0</v>
       </c>
       <c r="M60" s="19">
@@ -21866,7 +21866,7 @@
         <v>0</v>
       </c>
       <c r="P60" s="18">
-        <f t="shared" ref="P60:Q100" si="110">O60</f>
+        <f t="shared" ref="P60:Q94" si="110">O60</f>
         <v>0</v>
       </c>
       <c r="Q60" s="19">
@@ -21881,7 +21881,7 @@
         <v>3.5</v>
       </c>
       <c r="T60" s="18">
-        <f t="shared" ref="T60:U100" si="111">S60</f>
+        <f t="shared" ref="T60:U94" si="111">S60</f>
         <v>3.5</v>
       </c>
       <c r="U60" s="19">
@@ -21893,7 +21893,7 @@
         <v>0</v>
       </c>
       <c r="X60" s="18">
-        <f t="shared" ref="X60:Y100" si="112">W60</f>
+        <f t="shared" ref="X60:Y94" si="112">W60</f>
         <v>0</v>
       </c>
       <c r="Y60" s="19">
@@ -21905,7 +21905,7 @@
         <v>0</v>
       </c>
       <c r="AB60" s="18">
-        <f t="shared" ref="AB60:AC100" si="113">AA60</f>
+        <f t="shared" ref="AB60:AC94" si="113">AA60</f>
         <v>0</v>
       </c>
       <c r="AC60" s="19">
@@ -21919,7 +21919,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B61" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="9"/>
@@ -22009,10 +22009,10 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="10">
@@ -22103,7 +22103,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B63" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="9"/>
@@ -22124,7 +22124,7 @@
         <v>9.6</v>
       </c>
       <c r="K63" s="14">
-        <f t="shared" ref="K63:K103" si="114">J63</f>
+        <f t="shared" ref="K63:K80" si="114">J63</f>
         <v>0</v>
       </c>
       <c r="L63" s="18">
@@ -22136,7 +22136,7 @@
         <v>0</v>
       </c>
       <c r="O63" s="14">
-        <f t="shared" ref="O63:O103" si="115">N63</f>
+        <f t="shared" ref="O63:O80" si="115">N63</f>
         <v>0</v>
       </c>
       <c r="P63" s="18">
@@ -22151,7 +22151,7 @@
         <v>3.5</v>
       </c>
       <c r="S63" s="14">
-        <f t="shared" ref="S63:S103" si="116">R63</f>
+        <f t="shared" ref="S63:S80" si="116">R63</f>
         <v>3.5</v>
       </c>
       <c r="T63" s="18">
@@ -22166,7 +22166,7 @@
         <v>10</v>
       </c>
       <c r="W63" s="14">
-        <f t="shared" ref="W63:W103" si="117">V63</f>
+        <f t="shared" ref="W63:W80" si="117">V63</f>
         <v>10</v>
       </c>
       <c r="X63" s="18">
@@ -22181,7 +22181,7 @@
         <v>10</v>
       </c>
       <c r="AA63" s="14">
-        <f t="shared" ref="AA63:AA103" si="118">Z63</f>
+        <f t="shared" ref="AA63:AA80" si="118">Z63</f>
         <v>10</v>
       </c>
       <c r="AB63" s="18">
@@ -22199,7 +22199,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="9"/>
@@ -22295,12 +22295,12 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="9"/>
       <c r="E65" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F65" s="13">
         <v>115</v>
@@ -22393,7 +22393,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B66" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="9"/>
@@ -22477,7 +22477,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="9"/>
@@ -22561,7 +22561,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B68" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="9"/>
@@ -22645,7 +22645,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="9"/>
@@ -22747,7 +22747,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9"/>
@@ -22849,7 +22849,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B71" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="9"/>
@@ -22951,7 +22951,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="9"/>
@@ -23038,7 +23038,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="9"/>
@@ -23125,7 +23125,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="9"/>
@@ -23212,7 +23212,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="9"/>
@@ -23305,7 +23305,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="9"/>
@@ -23395,7 +23395,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="9"/>
@@ -23482,7 +23482,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B78" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="9"/>
@@ -23566,7 +23566,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B79" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9"/>
@@ -23653,7 +23653,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="9"/>
@@ -23740,7 +23740,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B81" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C81" s="5">
         <v>1.5</v>
@@ -23844,7 +23844,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C82" s="5">
         <v>1.5</v>
@@ -23948,7 +23948,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="9"/>
@@ -23966,7 +23966,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="14">
-        <f t="shared" ref="K83:K123" si="121">J83</f>
+        <f t="shared" ref="K83:K94" si="121">J83</f>
         <v>0</v>
       </c>
       <c r="L83" s="18">
@@ -23978,7 +23978,7 @@
         <v>0</v>
       </c>
       <c r="O83" s="14">
-        <f t="shared" ref="O83:O123" si="122">N83</f>
+        <f t="shared" ref="O83:O94" si="122">N83</f>
         <v>0</v>
       </c>
       <c r="P83" s="18">
@@ -23993,7 +23993,7 @@
         <v>2.5</v>
       </c>
       <c r="S83" s="14">
-        <f t="shared" ref="S83:S123" si="123">R83</f>
+        <f t="shared" ref="S83:S94" si="123">R83</f>
         <v>2.5</v>
       </c>
       <c r="T83" s="18">
@@ -24008,7 +24008,7 @@
         <v>1</v>
       </c>
       <c r="W83" s="14">
-        <f t="shared" ref="W83:W123" si="124">V83</f>
+        <f t="shared" ref="W83:W94" si="124">V83</f>
         <v>1</v>
       </c>
       <c r="X83" s="18">
@@ -24020,7 +24020,7 @@
         <v>1</v>
       </c>
       <c r="AA83" s="14">
-        <f t="shared" ref="AA83:AA123" si="125">Z83</f>
+        <f t="shared" ref="AA83:AA94" si="125">Z83</f>
         <v>0</v>
       </c>
       <c r="AB83" s="18">
@@ -24038,7 +24038,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="9"/>
@@ -24128,7 +24128,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B85" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="9"/>
@@ -24218,7 +24218,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B86" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="9"/>
@@ -24308,7 +24308,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B87" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="9"/>
@@ -24412,7 +24412,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B88" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="9"/>
@@ -24516,7 +24516,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="9"/>
@@ -24542,7 +24542,7 @@
         <v>0</v>
       </c>
       <c r="M89" s="19">
-        <f t="shared" ref="M89:M111" si="126">L89</f>
+        <f t="shared" ref="M89:M94" si="126">L89</f>
         <v>0</v>
       </c>
       <c r="O89" s="14">
@@ -24554,7 +24554,7 @@
         <v>0</v>
       </c>
       <c r="Q89" s="19">
-        <f t="shared" ref="Q89:Q111" si="127">P89</f>
+        <f t="shared" ref="Q89:Q94" si="127">P89</f>
         <v>0</v>
       </c>
       <c r="S89" s="14">
@@ -24566,7 +24566,7 @@
         <v>0</v>
       </c>
       <c r="U89" s="19">
-        <f t="shared" ref="U89:U111" si="128">T89</f>
+        <f t="shared" ref="U89:U94" si="128">T89</f>
         <v>0</v>
       </c>
       <c r="W89" s="14">
@@ -24578,7 +24578,7 @@
         <v>0</v>
       </c>
       <c r="Y89" s="19">
-        <f t="shared" ref="Y89:Y111" si="129">X89</f>
+        <f t="shared" ref="Y89:Y94" si="129">X89</f>
         <v>0</v>
       </c>
       <c r="AA89" s="14">
@@ -24590,7 +24590,7 @@
         <v>0</v>
       </c>
       <c r="AC89" s="19">
-        <f t="shared" ref="AC89:AC111" si="130">AB89</f>
+        <f t="shared" ref="AC89:AC94" si="130">AB89</f>
         <v>0</v>
       </c>
     </row>
@@ -24600,7 +24600,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="9"/>
@@ -24684,7 +24684,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B91" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="9"/>
@@ -24768,7 +24768,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B92" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="9"/>
@@ -24855,7 +24855,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B93" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="9"/>
@@ -24942,7 +24942,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B94" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="9"/>
@@ -25078,7 +25078,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>269</v>
@@ -25168,7 +25168,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C3" s="5">
         <v>0.33</v>
@@ -25266,7 +25266,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C4" s="5">
         <v>1.25</v>
@@ -25364,7 +25364,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C5" s="5">
         <v>1.5</v>
@@ -25462,7 +25462,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
@@ -25558,7 +25558,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C7" s="5">
         <v>0.25</v>
@@ -25656,7 +25656,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C8" s="5">
         <v>0.25</v>
@@ -25754,7 +25754,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C9" s="5">
         <v>1.25</v>
@@ -25843,7 +25843,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C10" s="5">
         <v>1.5</v>
@@ -25932,7 +25932,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -26019,7 +26019,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" s="5">
         <v>0.25</v>
@@ -26108,7 +26108,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C13" s="5">
         <v>0.25</v>
@@ -26197,7 +26197,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
@@ -26292,7 +26292,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C15" s="5">
         <v>0</v>
@@ -26387,7 +26387,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -26482,7 +26482,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C17" s="5">
         <v>0</v>
@@ -26577,7 +26577,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -26672,7 +26672,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -26762,7 +26762,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -26852,7 +26852,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -26942,7 +26942,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -27029,7 +27029,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -27116,7 +27116,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -27203,7 +27203,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -27290,7 +27290,7 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -27377,7 +27377,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -27470,7 +27470,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -27563,7 +27563,7 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -27656,7 +27656,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
@@ -27752,7 +27752,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
@@ -27848,7 +27848,7 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -27944,7 +27944,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -28034,7 +28034,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -28124,7 +28124,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9"/>
@@ -28226,7 +28226,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C36" s="5">
         <v>0.25</v>
@@ -28334,7 +28334,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B37" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C37" s="5">
         <v>0.25</v>
@@ -28440,7 +28440,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B38" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9"/>
@@ -28533,7 +28533,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C39" s="5">
         <v>0.25</v>
@@ -28632,7 +28632,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B40" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C40" s="5">
         <v>0.25</v>
@@ -28729,7 +28729,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9"/>
@@ -28828,7 +28828,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C42" s="5">
         <v>0.25</v>
@@ -28933,7 +28933,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B43" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C43" s="5">
         <v>0.25</v>
@@ -29038,7 +29038,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B44" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C44" s="5">
         <v>0.25</v>
@@ -29141,7 +29141,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="9"/>
@@ -29237,7 +29237,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C46" s="5">
         <v>0.25</v>
@@ -29339,7 +29339,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C47" s="5">
         <v>0.25</v>
@@ -29441,7 +29441,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C48" s="5">
         <v>0.25</v>
@@ -29541,7 +29541,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C49" s="5">
         <v>2</v>
@@ -29646,7 +29646,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" s="5">
         <v>2</v>
@@ -29751,7 +29751,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B51" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C51" s="5">
         <v>2</v>
@@ -29856,7 +29856,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C52" s="5">
         <v>2</v>
@@ -29961,7 +29961,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C53" s="5">
         <v>2</v>
@@ -30066,7 +30066,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6">
@@ -30167,7 +30167,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6">
@@ -30268,7 +30268,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="6">
@@ -30369,14 +30369,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F57" s="13">
         <v>5</v>
@@ -30466,14 +30466,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F58" s="13">
         <v>11</v>
@@ -30563,14 +30563,14 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F59" s="13">
         <v>0</v>
@@ -30660,7 +30660,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
@@ -30752,7 +30752,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B61" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
@@ -30844,10 +30844,10 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="7">
@@ -30938,7 +30938,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B63" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
@@ -31034,7 +31034,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
@@ -31130,12 +31130,12 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
       <c r="E65" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F65" s="13">
         <v>115</v>
@@ -31228,7 +31228,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B66" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
@@ -31312,7 +31312,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
@@ -31396,7 +31396,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B68" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
@@ -31480,7 +31480,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -31582,7 +31582,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
@@ -31684,7 +31684,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B71" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
@@ -31786,7 +31786,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
@@ -31873,7 +31873,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -31960,7 +31960,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
@@ -32047,7 +32047,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
@@ -32140,7 +32140,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -32230,7 +32230,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
@@ -32317,7 +32317,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B78" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
@@ -32401,7 +32401,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B79" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9"/>
@@ -32488,7 +32488,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="9"/>
@@ -32575,7 +32575,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B81" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C81" s="5">
         <v>1.75</v>
@@ -32679,7 +32679,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C82" s="5">
         <v>1.75</v>
@@ -32783,7 +32783,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="9"/>
@@ -32873,7 +32873,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="9"/>
@@ -32963,7 +32963,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B85" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
@@ -33053,7 +33053,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B86" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
@@ -33143,7 +33143,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B87" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
@@ -33247,7 +33247,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B88" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
@@ -33351,7 +33351,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -33435,7 +33435,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -33519,7 +33519,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B91" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
@@ -33603,7 +33603,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B92" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
@@ -33690,7 +33690,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B93" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
@@ -33777,7 +33777,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B94" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>

</xml_diff>

<commit_message>
Updated all scripts to exclude verbose specs that must be hard coded. Added |.
</commit_message>
<xml_diff>
--- a/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
+++ b/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
@@ -1380,39 +1380,6 @@
     <t xml:space="preserve"> * = 1.25</t>
   </si>
   <si>
-    <t xml:space="preserve"> + = SWood_1000hr * 0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SWood_10_000hr * 0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SWood_GT10_000hr * 0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SWood_1000hr * 0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SWood_10_000hr * 0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SWood_GT10_000hr * 0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = SStump_Density</t>
-  </si>
-  <si>
-    <t>MAKE EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = 0.75*OTree_Density + 0.75*MTree_Density</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = 0.5*OTree_Density + 0.5*MTree_Density</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + = 0.25*OTree_Density + 0.25*MTree_Density</t>
-  </si>
-  <si>
     <t xml:space="preserve"> * = 1/0.5</t>
   </si>
   <si>
@@ -1588,6 +1555,39 @@
   </si>
   <si>
     <t>FB_0291_FCCS_233</t>
+  </si>
+  <si>
+    <t>| + = SWood_1000hr * 0.25</t>
+  </si>
+  <si>
+    <t>| + = SWood_10_000hr * 0.25</t>
+  </si>
+  <si>
+    <t>| + = SWood_GT10_000hr * 0.25</t>
+  </si>
+  <si>
+    <t>| + = SWood_1000hr * 0.5</t>
+  </si>
+  <si>
+    <t>| + = SWood_10_000hr * 0.5</t>
+  </si>
+  <si>
+    <t>| + = SWood_GT10_000hr * 0.5</t>
+  </si>
+  <si>
+    <t>| = 0</t>
+  </si>
+  <si>
+    <t>| + = 0.25*OTree_Density + 0.25*MTree_Density</t>
+  </si>
+  <si>
+    <t>| + = 0.5*OTree_Density + 0.5*MTree_Density</t>
+  </si>
+  <si>
+    <t>| + = 0.75*OTree_Density + 0.75*MTree_Density</t>
+  </si>
+  <si>
+    <t>| + = SStump_Density</t>
   </si>
 </sst>
 </file>
@@ -2659,7 +2659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K100" sqref="K100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3155,21 +3157,21 @@
         <v>271</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="21" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="22" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="K36" s="23"/>
     </row>
@@ -3230,14 +3232,14 @@
         <v>271</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="E39" s="23"/>
       <c r="F39" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="21" t="s">
@@ -3341,20 +3343,20 @@
         <v>270</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="E43" s="23"/>
       <c r="F43" s="21" t="s">
         <v>271</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>1</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="K43" s="23"/>
     </row>
@@ -3444,19 +3446,19 @@
         <v>270</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>271</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="I47" s="21" t="s">
         <v>1</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="K47" s="23"/>
     </row>
@@ -3697,22 +3699,22 @@
         <v>341</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>377</v>
+        <v>436</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>380</v>
+        <v>439</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>377</v>
+        <v>436</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>380</v>
+        <v>439</v>
       </c>
       <c r="J56" s="33" t="s">
-        <v>377</v>
+        <v>436</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>380</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3723,22 +3725,22 @@
         <v>342</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>378</v>
+        <v>437</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>381</v>
+        <v>440</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>378</v>
+        <v>437</v>
       </c>
       <c r="H57" s="23" t="s">
-        <v>381</v>
+        <v>440</v>
       </c>
       <c r="J57" s="33" t="s">
-        <v>378</v>
+        <v>437</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>381</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3749,22 +3751,22 @@
         <v>343</v>
       </c>
       <c r="D58" s="33" t="s">
-        <v>379</v>
+        <v>438</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>382</v>
+        <v>441</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>379</v>
+        <v>438</v>
       </c>
       <c r="H58" s="23" t="s">
-        <v>382</v>
+        <v>441</v>
       </c>
       <c r="J58" s="33" t="s">
-        <v>379</v>
+        <v>438</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>382</v>
+        <v>441</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3791,22 +3793,22 @@
         <v>346</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>384</v>
+        <v>442</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>386</v>
+        <v>444</v>
       </c>
       <c r="H61" s="23" t="s">
-        <v>384</v>
+        <v>442</v>
       </c>
       <c r="I61" s="21" t="s">
-        <v>385</v>
+        <v>445</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>384</v>
+        <v>442</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3833,13 +3835,13 @@
         <v>349</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>383</v>
+        <v>446</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>383</v>
+        <v>446</v>
       </c>
       <c r="K64" s="23" t="s">
-        <v>383</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -7502,73 +7504,73 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="H1" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="I1" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="L1" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="M1" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="P1" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="Q1" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
       </c>
       <c r="S1" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="T1" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="U1" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="V1" t="s">
         <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="X1" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="Y1" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="Z1" t="s">
         <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="AB1" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="AC1" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -16318,73 +16320,73 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="H1" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="I1" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="L1" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="M1" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="P1" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="Q1" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
       </c>
       <c r="S1" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="T1" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="U1" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="V1" t="s">
         <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="X1" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="Y1" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="Z1" t="s">
         <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="AB1" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="AC1" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -25133,73 +25135,73 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="H1" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="I1" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="L1" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="M1" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="P1" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="Q1" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
       </c>
       <c r="S1" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="T1" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="U1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="V1" t="s">
         <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="X1" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="Y1" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="Z1" t="s">
         <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="AB1" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="AC1" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated mech add and mech remove scripts for rotten wood
</commit_message>
<xml_diff>
--- a/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
+++ b/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="452">
   <si>
     <t>* = 1.1</t>
   </si>
@@ -1598,6 +1598,12 @@
   <si>
     <t>| if = 0, but add SStump, = SStump_Density</t>
   </si>
+  <si>
+    <t>| If not present, Sstump_Diameter</t>
+  </si>
+  <si>
+    <t>| If not present, Sstump_Height</t>
+  </si>
 </sst>
 </file>
 
@@ -2668,20 +2674,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.42578125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="21" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="25" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="26" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="21" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="25" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="26" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="26" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" style="21" customWidth="1"/>
     <col min="10" max="10" width="26.5703125" style="25" customWidth="1"/>
     <col min="11" max="11" width="26.5703125" style="26" customWidth="1"/>
@@ -3833,6 +3839,15 @@
       <c r="B62" t="s">
         <v>346</v>
       </c>
+      <c r="E62" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="K62" s="23" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
@@ -3841,6 +3856,15 @@
       <c r="B63" t="s">
         <v>347</v>
       </c>
+      <c r="E63" s="23" t="s">
+        <v>451</v>
+      </c>
+      <c r="H63" s="23" t="s">
+        <v>451</v>
+      </c>
+      <c r="K63" s="23" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
@@ -3866,9 +3890,6 @@
       <c r="B65" t="s">
         <v>346</v>
       </c>
-      <c r="E65" s="23" t="s">
-        <v>447</v>
-      </c>
       <c r="H65" s="23" t="s">
         <v>447</v>
       </c>
@@ -3883,9 +3904,6 @@
       <c r="B66" t="s">
         <v>347</v>
       </c>
-      <c r="E66" s="23" t="s">
-        <v>448</v>
-      </c>
       <c r="H66" s="23" t="s">
         <v>448</v>
       </c>
@@ -3900,9 +3918,7 @@
       <c r="B67" t="s">
         <v>348</v>
       </c>
-      <c r="E67" s="23" t="s">
-        <v>449</v>
-      </c>
+      <c r="E67" s="23"/>
       <c r="H67" s="23" t="s">
         <v>449</v>
       </c>
@@ -7504,8 +7520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView topLeftCell="U1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7936,7 +7952,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5:K15" si="8">J5</f>
+        <f t="shared" ref="K5" si="8">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -7948,7 +7964,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5:O15" si="10">N5</f>
+        <f t="shared" ref="O5" si="10">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -7963,7 +7979,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5:S15" si="12">R5</f>
+        <f t="shared" ref="S5" si="12">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -7978,7 +7994,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5:W15" si="14">V5</f>
+        <f t="shared" ref="W5" si="14">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -7993,7 +8009,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5:AA15" si="16">Z5</f>
+        <f t="shared" ref="AA5" si="16">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -8403,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10:K20" si="18">J10</f>
+        <f t="shared" ref="K10" si="18">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -8415,7 +8431,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10:O20" si="19">N10</f>
+        <f t="shared" ref="O10" si="19">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -8427,7 +8443,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10:S20" si="20">R10</f>
+        <f t="shared" ref="S10" si="20">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -8442,7 +8458,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10:W20" si="21">V10</f>
+        <f t="shared" ref="W10" si="21">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -8454,7 +8470,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10:AA20" si="22">Z10</f>
+        <f t="shared" ref="AA10" si="22">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -8668,7 +8684,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" ref="K13:K23" si="23">J13</f>
+        <f t="shared" ref="K13:K15" si="23">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
@@ -8680,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" ref="O13:O23" si="24">N13</f>
+        <f t="shared" ref="O13:O15" si="24">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
@@ -8695,7 +8711,7 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" ref="S13:S23" si="25">R13</f>
+        <f t="shared" ref="S13:S15" si="25">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="15">
@@ -8710,7 +8726,7 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="12">
-        <f t="shared" ref="W13:W23" si="26">V13</f>
+        <f t="shared" ref="W13:W15" si="26">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="15">
@@ -8725,7 +8741,7 @@
         <v>1</v>
       </c>
       <c r="AA13" s="12">
-        <f t="shared" ref="AA13:AA23" si="27">Z13</f>
+        <f t="shared" ref="AA13:AA15" si="27">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="15">
@@ -10603,7 +10619,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34:M47" si="36">L34</f>
+        <f t="shared" ref="M34" si="36">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -10618,7 +10634,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34:Q47" si="37">P34</f>
+        <f t="shared" ref="Q34" si="37">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -10633,7 +10649,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34:U47" si="38">T34</f>
+        <f t="shared" ref="U34" si="38">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -10648,7 +10664,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34:Y47" si="39">X34</f>
+        <f t="shared" ref="Y34" si="39">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -10663,7 +10679,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34:AC47" si="40">AB34</f>
+        <f t="shared" ref="AC34" si="40">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -10912,66 +10928,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37:K44" si="43">J37</f>
+        <f t="shared" ref="K37" si="43">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37:L44" si="44">K37</f>
+        <f t="shared" ref="L37" si="44">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37:M50" si="45">L37</f>
+        <f t="shared" ref="M37" si="45">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37:O44" si="46">N37</f>
+        <f t="shared" ref="O37" si="46">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37:P44" si="47">O37</f>
+        <f t="shared" ref="P37" si="47">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37:Q50" si="48">P37</f>
+        <f t="shared" ref="Q37" si="48">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37:S44" si="49">R37</f>
+        <f t="shared" ref="S37" si="49">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37:T44" si="50">S37</f>
+        <f t="shared" ref="T37" si="50">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37:U50" si="51">T37</f>
+        <f t="shared" ref="U37" si="51">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37:W44" si="52">V37</f>
+        <f t="shared" ref="W37" si="52">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37:X44" si="53">W37</f>
+        <f t="shared" ref="X37" si="53">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37:Y50" si="54">X37</f>
+        <f t="shared" ref="Y37" si="54">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37:AA44" si="55">Z37</f>
+        <f t="shared" ref="AA37" si="55">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37:AB44" si="56">AA37</f>
+        <f t="shared" ref="AB37" si="56">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37:AC50" si="57">AB37</f>
+        <f t="shared" ref="AC37" si="57">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -11199,75 +11215,75 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40:K47" si="58">J40</f>
+        <f t="shared" ref="K40" si="58">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40:L47" si="59">K40</f>
+        <f t="shared" ref="L40" si="59">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" ref="M40:M53" si="60">L40</f>
+        <f t="shared" ref="M40" si="60">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="11">
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40:O47" si="61">N40</f>
+        <f t="shared" ref="O40" si="61">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40:P47" si="62">O40</f>
+        <f t="shared" ref="P40" si="62">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
-        <f t="shared" ref="Q40:Q53" si="63">P40</f>
+        <f t="shared" ref="Q40" si="63">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="11">
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40:S47" si="64">R40</f>
+        <f t="shared" ref="S40" si="64">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40:T47" si="65">S40</f>
+        <f t="shared" ref="T40" si="65">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" ref="U40:U53" si="66">T40</f>
+        <f t="shared" ref="U40" si="66">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="11">
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40:W47" si="67">V40</f>
+        <f t="shared" ref="W40" si="67">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40:X47" si="68">W40</f>
+        <f t="shared" ref="X40" si="68">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
-        <f t="shared" ref="Y40:Y53" si="69">X40</f>
+        <f t="shared" ref="Y40" si="69">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="11">
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40:AA47" si="70">Z40</f>
+        <f t="shared" ref="AA40" si="70">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40:AB47" si="71">AA40</f>
+        <f t="shared" ref="AB40" si="71">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
-        <f t="shared" ref="AC40:AC53" si="72">AB40</f>
+        <f t="shared" ref="AC40" si="72">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -11521,7 +11537,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M56" si="73">L43</f>
+        <f t="shared" ref="M43:M44" si="73">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -11536,7 +11552,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q56" si="74">P43</f>
+        <f t="shared" ref="Q43:Q44" si="74">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -11551,7 +11567,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U56" si="75">T43</f>
+        <f t="shared" ref="U43:U44" si="75">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -11566,7 +11582,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y56" si="76">X43</f>
+        <f t="shared" ref="Y43:Y44" si="76">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -11581,7 +11597,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC56" si="77">AB43</f>
+        <f t="shared" ref="AC43:AC44" si="77">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -11612,11 +11628,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44:K51" si="78">J44</f>
+        <f t="shared" ref="K44" si="78">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44:L51" si="79">K44</f>
+        <f t="shared" ref="L44" si="79">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -11627,11 +11643,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44:O51" si="80">N44</f>
+        <f t="shared" ref="O44" si="80">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44:P51" si="81">O44</f>
+        <f t="shared" ref="P44" si="81">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -11642,11 +11658,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44:S51" si="82">R44</f>
+        <f t="shared" ref="S44" si="82">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44:T51" si="83">S44</f>
+        <f t="shared" ref="T44" si="83">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -11654,11 +11670,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44:W51" si="84">V44</f>
+        <f t="shared" ref="W44" si="84">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44:X51" si="85">W44</f>
+        <f t="shared" ref="X44" si="85">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -11669,11 +11685,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44:AA51" si="86">Z44</f>
+        <f t="shared" ref="AA44" si="86">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44:AB51" si="87">AA44</f>
+        <f t="shared" ref="AB44" si="87">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -11718,7 +11734,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="15">
-        <f t="shared" ref="L45:L55" si="89">K45*$D45</f>
+        <f t="shared" ref="L45" si="89">K45*$D45</f>
         <v>0</v>
       </c>
       <c r="M45" s="16">
@@ -11733,7 +11749,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" ref="P45:P55" si="90">O45*$D45</f>
+        <f t="shared" ref="P45" si="90">O45*$D45</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="Q45" s="16">
@@ -11748,7 +11764,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="T45" s="15">
-        <f t="shared" ref="T45:T55" si="91">S45*$D45</f>
+        <f t="shared" ref="T45" si="91">S45*$D45</f>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="U45" s="16">
@@ -11760,7 +11776,7 @@
         <v>0</v>
       </c>
       <c r="X45" s="15">
-        <f t="shared" ref="X45:X55" si="92">W45*$D45</f>
+        <f t="shared" ref="X45" si="92">W45*$D45</f>
         <v>0</v>
       </c>
       <c r="Y45" s="16">
@@ -11775,7 +11791,7 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="AB45" s="15">
-        <f t="shared" ref="AB45:AB55" si="93">AA45*$D45</f>
+        <f t="shared" ref="AB45" si="93">AA45*$D45</f>
         <v>9.3750000000000014E-2</v>
       </c>
       <c r="AC45" s="16">
@@ -11921,11 +11937,11 @@
         <v>0</v>
       </c>
       <c r="L47" s="15">
-        <f t="shared" ref="L47:L57" si="94">K47*$D47</f>
+        <f t="shared" ref="L47:L48" si="94">K47*$D47</f>
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47:M60" si="95">L47</f>
+        <f t="shared" ref="M47" si="95">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -11936,11 +11952,11 @@
         <v>52.5</v>
       </c>
       <c r="P47" s="15">
-        <f t="shared" ref="P47:P57" si="96">O47*$D47</f>
+        <f t="shared" ref="P47:P48" si="96">O47*$D47</f>
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47:Q60" si="97">P47</f>
+        <f t="shared" ref="Q47" si="97">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -11951,11 +11967,11 @@
         <v>67.5</v>
       </c>
       <c r="T47" s="15">
-        <f t="shared" ref="T47:T57" si="98">S47*$D47</f>
+        <f t="shared" ref="T47:T48" si="98">S47*$D47</f>
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47:U60" si="99">T47</f>
+        <f t="shared" ref="U47" si="99">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -11963,11 +11979,11 @@
         <v>0</v>
       </c>
       <c r="X47" s="15">
-        <f t="shared" ref="X47:X57" si="100">W47*$D47</f>
+        <f t="shared" ref="X47:X48" si="100">W47*$D47</f>
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47:Y60" si="101">X47</f>
+        <f t="shared" ref="Y47" si="101">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -11978,11 +11994,11 @@
         <v>45</v>
       </c>
       <c r="AB47" s="15">
-        <f t="shared" ref="AB47:AB57" si="102">AA47*$D47</f>
+        <f t="shared" ref="AB47:AB48" si="102">AA47*$D47</f>
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47:AC60" si="103">AB47</f>
+        <f t="shared" ref="AC47" si="103">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -12030,7 +12046,7 @@
         <v>0.9375</v>
       </c>
       <c r="M48" s="16">
-        <f t="shared" ref="M48:M52" si="105">$E48*L48</f>
+        <f t="shared" ref="M48" si="105">$E48*L48</f>
         <v>0.46875</v>
       </c>
       <c r="O48" s="12">
@@ -12042,7 +12058,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="16">
-        <f t="shared" ref="Q48:Q52" si="106">$E48*P48</f>
+        <f t="shared" ref="Q48" si="106">$E48*P48</f>
         <v>0</v>
       </c>
       <c r="R48" s="11">
@@ -12057,7 +12073,7 @@
         <v>0.46875</v>
       </c>
       <c r="U48" s="16">
-        <f t="shared" ref="U48:U52" si="107">$E48*T48</f>
+        <f t="shared" ref="U48" si="107">$E48*T48</f>
         <v>0.234375</v>
       </c>
       <c r="V48" s="11">
@@ -12072,7 +12088,7 @@
         <v>0.9375</v>
       </c>
       <c r="Y48" s="16">
-        <f t="shared" ref="Y48:Y52" si="108">$E48*X48</f>
+        <f t="shared" ref="Y48" si="108">$E48*X48</f>
         <v>0.46875</v>
       </c>
       <c r="Z48" s="11">
@@ -12087,7 +12103,7 @@
         <v>0.46875</v>
       </c>
       <c r="AC48" s="16">
-        <f t="shared" ref="AC48:AC52" si="109">$E48*AB48</f>
+        <f t="shared" ref="AC48" si="109">$E48*AB48</f>
         <v>0.234375</v>
       </c>
     </row>
@@ -12236,7 +12252,7 @@
         <v>1.25</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" ref="L50:L60" si="110">K50*$D50</f>
+        <f t="shared" ref="L50:L52" si="110">K50*$D50</f>
         <v>0.9375</v>
       </c>
       <c r="M50" s="16">
@@ -12248,7 +12264,7 @@
         <v>0.5</v>
       </c>
       <c r="P50" s="15">
-        <f t="shared" ref="P50:P60" si="112">O50*$D50</f>
+        <f t="shared" ref="P50:P52" si="112">O50*$D50</f>
         <v>0.375</v>
       </c>
       <c r="Q50" s="16">
@@ -12263,7 +12279,7 @@
         <v>0.625</v>
       </c>
       <c r="T50" s="15">
-        <f t="shared" ref="T50:T60" si="114">S50*$D50</f>
+        <f t="shared" ref="T50:T52" si="114">S50*$D50</f>
         <v>0.46875</v>
       </c>
       <c r="U50" s="16">
@@ -12278,7 +12294,7 @@
         <v>1.25</v>
       </c>
       <c r="X50" s="15">
-        <f t="shared" ref="X50:X60" si="116">W50*$D50</f>
+        <f t="shared" ref="X50:X52" si="116">W50*$D50</f>
         <v>0.9375</v>
       </c>
       <c r="Y50" s="16">
@@ -12293,7 +12309,7 @@
         <v>0.5</v>
       </c>
       <c r="AB50" s="15">
-        <f t="shared" ref="AB50:AB60" si="118">AA50*$D50</f>
+        <f t="shared" ref="AB50:AB52" si="118">AA50*$D50</f>
         <v>0.375</v>
       </c>
       <c r="AC50" s="16">
@@ -12545,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" ref="K53:K93" si="122">J53</f>
+        <f t="shared" ref="K53:K60" si="122">J53</f>
         <v>0</v>
       </c>
       <c r="L53" s="15">
@@ -12557,7 +12573,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="12">
-        <f t="shared" ref="O53:O93" si="123">N53</f>
+        <f t="shared" ref="O53:O60" si="123">N53</f>
         <v>0</v>
       </c>
       <c r="P53" s="15">
@@ -12572,7 +12588,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="12">
-        <f t="shared" ref="S53:S93" si="124">R53</f>
+        <f t="shared" ref="S53:S60" si="124">R53</f>
         <v>1</v>
       </c>
       <c r="T53" s="15">
@@ -12587,7 +12603,7 @@
         <v>1.2</v>
       </c>
       <c r="W53" s="12">
-        <f t="shared" ref="W53:W93" si="125">V53</f>
+        <f t="shared" ref="W53:W60" si="125">V53</f>
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
@@ -12602,7 +12618,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53" s="12">
-        <f t="shared" ref="AA53:AA93" si="126">Z53</f>
+        <f t="shared" ref="AA53:AA60" si="126">Z53</f>
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
@@ -12652,7 +12668,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="15">
-        <f t="shared" ref="L54:L64" si="127">K54*$D54</f>
+        <f t="shared" ref="L54:L55" si="127">K54*$D54</f>
         <v>0</v>
       </c>
       <c r="M54" s="16">
@@ -12664,7 +12680,7 @@
         <v>0</v>
       </c>
       <c r="P54" s="15">
-        <f t="shared" ref="P54:P64" si="128">O54*$D54</f>
+        <f t="shared" ref="P54:P55" si="128">O54*$D54</f>
         <v>0</v>
       </c>
       <c r="Q54" s="16">
@@ -12679,7 +12695,7 @@
         <v>0</v>
       </c>
       <c r="T54" s="15">
-        <f t="shared" ref="T54:T64" si="129">S54*$D54</f>
+        <f t="shared" ref="T54:T55" si="129">S54*$D54</f>
         <v>0</v>
       </c>
       <c r="U54" s="16">
@@ -12694,7 +12710,7 @@
         <v>0.5</v>
       </c>
       <c r="X54" s="15">
-        <f t="shared" ref="X54:X64" si="130">W54*$D54</f>
+        <f t="shared" ref="X54:X55" si="130">W54*$D54</f>
         <v>0.375</v>
       </c>
       <c r="Y54" s="16">
@@ -12709,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="15">
-        <f t="shared" ref="AB54:AB64" si="131">AA54*$D54</f>
+        <f t="shared" ref="AB54:AB55" si="131">AA54*$D54</f>
         <v>0</v>
       </c>
       <c r="AC54" s="16">
@@ -13416,7 +13432,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K93" si="138">J62</f>
+        <f t="shared" ref="K62:K79" si="138">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -13428,7 +13444,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O93" si="140">N62</f>
+        <f t="shared" ref="O62:O79" si="140">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -13443,7 +13459,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S93" si="142">R62</f>
+        <f t="shared" ref="S62:S79" si="142">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -13458,7 +13474,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W93" si="144">V62</f>
+        <f t="shared" ref="W62:W79" si="144">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -13473,7 +13489,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA93" si="146">Z62</f>
+        <f t="shared" ref="AA62:AA79" si="146">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -16750,7 +16766,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5:K20" si="7">J5</f>
+        <f t="shared" ref="K5" si="7">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -16762,7 +16778,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5:O20" si="9">N5</f>
+        <f t="shared" ref="O5" si="9">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -16777,7 +16793,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5:S20" si="11">R5</f>
+        <f t="shared" ref="S5" si="11">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -16792,7 +16808,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5:W20" si="13">V5</f>
+        <f t="shared" ref="W5" si="13">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -16807,7 +16823,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5:AA20" si="15">Z5</f>
+        <f t="shared" ref="AA5" si="15">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -17217,7 +17233,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10:K25" si="17">J10</f>
+        <f t="shared" ref="K10" si="17">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -17229,7 +17245,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10:O25" si="18">N10</f>
+        <f t="shared" ref="O10" si="18">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -17241,7 +17257,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10:S25" si="19">R10</f>
+        <f t="shared" ref="S10" si="19">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -17256,7 +17272,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10:W25" si="20">V10</f>
+        <f t="shared" ref="W10" si="20">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -17268,7 +17284,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10:AA25" si="21">Z10</f>
+        <f t="shared" ref="AA10" si="21">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -19732,66 +19748,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37:K44" si="36">J37</f>
+        <f t="shared" ref="K37" si="36">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37:L44" si="37">K37</f>
+        <f t="shared" ref="L37" si="37">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37:M50" si="38">L37</f>
+        <f t="shared" ref="M37" si="38">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37:O44" si="39">N37</f>
+        <f t="shared" ref="O37" si="39">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37:P44" si="40">O37</f>
+        <f t="shared" ref="P37" si="40">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37:Q50" si="41">P37</f>
+        <f t="shared" ref="Q37" si="41">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37:S44" si="42">R37</f>
+        <f t="shared" ref="S37" si="42">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37:T44" si="43">S37</f>
+        <f t="shared" ref="T37" si="43">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37:U50" si="44">T37</f>
+        <f t="shared" ref="U37" si="44">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37:W44" si="45">V37</f>
+        <f t="shared" ref="W37" si="45">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37:X44" si="46">W37</f>
+        <f t="shared" ref="X37" si="46">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37:Y50" si="47">X37</f>
+        <f t="shared" ref="Y37" si="47">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37:AA44" si="48">Z37</f>
+        <f t="shared" ref="AA37" si="48">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37:AB44" si="49">AA37</f>
+        <f t="shared" ref="AB37" si="49">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37:AC50" si="50">AB37</f>
+        <f t="shared" ref="AC37" si="50">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -20019,75 +20035,75 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40:K47" si="51">J40</f>
+        <f t="shared" ref="K40" si="51">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40:L47" si="52">K40</f>
+        <f t="shared" ref="L40" si="52">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" ref="M40:M53" si="53">L40</f>
+        <f t="shared" ref="M40" si="53">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="11">
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40:O47" si="54">N40</f>
+        <f t="shared" ref="O40" si="54">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40:P47" si="55">O40</f>
+        <f t="shared" ref="P40" si="55">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
-        <f t="shared" ref="Q40:Q53" si="56">P40</f>
+        <f t="shared" ref="Q40" si="56">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="11">
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40:S47" si="57">R40</f>
+        <f t="shared" ref="S40" si="57">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40:T47" si="58">S40</f>
+        <f t="shared" ref="T40" si="58">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" ref="U40:U53" si="59">T40</f>
+        <f t="shared" ref="U40" si="59">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="11">
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40:W47" si="60">V40</f>
+        <f t="shared" ref="W40" si="60">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40:X47" si="61">W40</f>
+        <f t="shared" ref="X40" si="61">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
-        <f t="shared" ref="Y40:Y53" si="62">X40</f>
+        <f t="shared" ref="Y40" si="62">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="11">
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40:AA47" si="63">Z40</f>
+        <f t="shared" ref="AA40" si="63">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40:AB47" si="64">AA40</f>
+        <f t="shared" ref="AB40" si="64">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
-        <f t="shared" ref="AC40:AC53" si="65">AB40</f>
+        <f t="shared" ref="AC40" si="65">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -20341,7 +20357,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M56" si="66">L43</f>
+        <f t="shared" ref="M43:M44" si="66">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -20356,7 +20372,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q56" si="67">P43</f>
+        <f t="shared" ref="Q43:Q44" si="67">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -20371,7 +20387,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U56" si="68">T43</f>
+        <f t="shared" ref="U43:U44" si="68">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -20386,7 +20402,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y56" si="69">X43</f>
+        <f t="shared" ref="Y43:Y44" si="69">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -20401,7 +20417,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC56" si="70">AB43</f>
+        <f t="shared" ref="AC43:AC44" si="70">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -20432,11 +20448,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44:K51" si="71">J44</f>
+        <f t="shared" ref="K44" si="71">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44:L51" si="72">K44</f>
+        <f t="shared" ref="L44" si="72">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -20447,11 +20463,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44:O51" si="73">N44</f>
+        <f t="shared" ref="O44" si="73">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44:P51" si="74">O44</f>
+        <f t="shared" ref="P44" si="74">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -20462,11 +20478,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44:S51" si="75">R44</f>
+        <f t="shared" ref="S44" si="75">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44:T51" si="76">S44</f>
+        <f t="shared" ref="T44" si="76">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -20474,11 +20490,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44:W51" si="77">V44</f>
+        <f t="shared" ref="W44" si="77">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44:X51" si="78">W44</f>
+        <f t="shared" ref="X44" si="78">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -20489,11 +20505,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44:AA51" si="79">Z44</f>
+        <f t="shared" ref="AA44" si="79">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44:AB51" si="80">AA44</f>
+        <f t="shared" ref="AB44" si="80">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -20538,7 +20554,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="15">
-        <f t="shared" ref="L45:L55" si="82">K45*$D45</f>
+        <f t="shared" ref="L45" si="82">K45*$D45</f>
         <v>0</v>
       </c>
       <c r="M45" s="16">
@@ -20553,7 +20569,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" ref="P45:P55" si="83">O45*$D45</f>
+        <f t="shared" ref="P45" si="83">O45*$D45</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="Q45" s="16">
@@ -20568,7 +20584,7 @@
         <v>0.01</v>
       </c>
       <c r="T45" s="15">
-        <f t="shared" ref="T45:T55" si="84">S45*$D45</f>
+        <f t="shared" ref="T45" si="84">S45*$D45</f>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="U45" s="16">
@@ -20580,7 +20596,7 @@
         <v>0</v>
       </c>
       <c r="X45" s="15">
-        <f t="shared" ref="X45:X55" si="85">W45*$D45</f>
+        <f t="shared" ref="X45" si="85">W45*$D45</f>
         <v>0</v>
       </c>
       <c r="Y45" s="16">
@@ -20595,7 +20611,7 @@
         <v>0.05</v>
       </c>
       <c r="AB45" s="15">
-        <f t="shared" ref="AB45:AB55" si="86">AA45*$D45</f>
+        <f t="shared" ref="AB45" si="86">AA45*$D45</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="AC45" s="16">
@@ -20745,7 +20761,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47:M60" si="87">L47</f>
+        <f t="shared" ref="M47" si="87">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -20760,7 +20776,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47:Q60" si="88">P47</f>
+        <f t="shared" ref="Q47" si="88">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -20775,7 +20791,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47:U60" si="89">T47</f>
+        <f t="shared" ref="U47" si="89">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -20787,7 +20803,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47:Y60" si="90">X47</f>
+        <f t="shared" ref="Y47" si="90">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -20802,7 +20818,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47:AC60" si="91">AB47</f>
+        <f t="shared" ref="AC47" si="91">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -20846,7 +20862,7 @@
         <v>1.5</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" ref="L48:L58" si="92">K48*$D48</f>
+        <f t="shared" ref="L48" si="92">K48*$D48</f>
         <v>1.125</v>
       </c>
       <c r="M48" s="16">
@@ -20858,7 +20874,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="15">
-        <f t="shared" ref="P48:P58" si="93">O48*$D48</f>
+        <f t="shared" ref="P48" si="93">O48*$D48</f>
         <v>0</v>
       </c>
       <c r="Q48" s="16">
@@ -20873,7 +20889,7 @@
         <v>0.75</v>
       </c>
       <c r="T48" s="15">
-        <f t="shared" ref="T48:T58" si="94">S48*$D48</f>
+        <f t="shared" ref="T48" si="94">S48*$D48</f>
         <v>0.5625</v>
       </c>
       <c r="U48" s="16">
@@ -20888,7 +20904,7 @@
         <v>1.5</v>
       </c>
       <c r="X48" s="15">
-        <f t="shared" ref="X48:X58" si="95">W48*$D48</f>
+        <f t="shared" ref="X48" si="95">W48*$D48</f>
         <v>1.125</v>
       </c>
       <c r="Y48" s="16">
@@ -20903,7 +20919,7 @@
         <v>0.75</v>
       </c>
       <c r="AB48" s="15">
-        <f t="shared" ref="AB48:AB58" si="96">AA48*$D48</f>
+        <f t="shared" ref="AB48" si="96">AA48*$D48</f>
         <v>0.5625</v>
       </c>
       <c r="AC48" s="16">
@@ -21056,7 +21072,7 @@
         <v>1.5</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" ref="L50:L60" si="97">K50*$D50</f>
+        <f t="shared" ref="L50:L55" si="97">K50*$D50</f>
         <v>1.125</v>
       </c>
       <c r="M50" s="16">
@@ -21068,7 +21084,7 @@
         <v>1</v>
       </c>
       <c r="P50" s="15">
-        <f t="shared" ref="P50:P60" si="98">O50*$D50</f>
+        <f t="shared" ref="P50:P55" si="98">O50*$D50</f>
         <v>0.75</v>
       </c>
       <c r="Q50" s="16">
@@ -21083,7 +21099,7 @@
         <v>1</v>
       </c>
       <c r="T50" s="15">
-        <f t="shared" ref="T50:T60" si="99">S50*$D50</f>
+        <f t="shared" ref="T50:T55" si="99">S50*$D50</f>
         <v>0.75</v>
       </c>
       <c r="U50" s="16">
@@ -21098,7 +21114,7 @@
         <v>1.5</v>
       </c>
       <c r="X50" s="15">
-        <f t="shared" ref="X50:X60" si="100">W50*$D50</f>
+        <f t="shared" ref="X50:X55" si="100">W50*$D50</f>
         <v>1.125</v>
       </c>
       <c r="Y50" s="16">
@@ -21113,7 +21129,7 @@
         <v>1</v>
       </c>
       <c r="AB50" s="15">
-        <f t="shared" ref="AB50:AB60" si="101">AA50*$D50</f>
+        <f t="shared" ref="AB50:AB55" si="101">AA50*$D50</f>
         <v>0.75</v>
       </c>
       <c r="AC50" s="16">
@@ -21363,7 +21379,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" ref="K53:K93" si="103">J53</f>
+        <f t="shared" ref="K53:K60" si="103">J53</f>
         <v>0</v>
       </c>
       <c r="L53" s="15">
@@ -21375,7 +21391,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="12">
-        <f t="shared" ref="O53:O93" si="104">N53</f>
+        <f t="shared" ref="O53:O60" si="104">N53</f>
         <v>0</v>
       </c>
       <c r="P53" s="15">
@@ -21390,7 +21406,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="12">
-        <f t="shared" ref="S53:S93" si="105">R53</f>
+        <f t="shared" ref="S53:S60" si="105">R53</f>
         <v>1</v>
       </c>
       <c r="T53" s="15">
@@ -21405,7 +21421,7 @@
         <v>1.2</v>
       </c>
       <c r="W53" s="12">
-        <f t="shared" ref="W53:W93" si="106">V53</f>
+        <f t="shared" ref="W53:W60" si="106">V53</f>
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
@@ -21420,7 +21436,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53" s="12">
-        <f t="shared" ref="AA53:AA93" si="107">Z53</f>
+        <f t="shared" ref="AA53:AA60" si="107">Z53</f>
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
@@ -22226,7 +22242,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K93" si="113">J62</f>
+        <f t="shared" ref="K62:K79" si="113">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -22238,7 +22254,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O93" si="114">N62</f>
+        <f t="shared" ref="O62:O79" si="114">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -22253,7 +22269,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S93" si="115">R62</f>
+        <f t="shared" ref="S62:S79" si="115">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -22268,7 +22284,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W93" si="116">V62</f>
+        <f t="shared" ref="W62:W79" si="116">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -22283,7 +22299,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA93" si="117">Z62</f>
+        <f t="shared" ref="AA62:AA79" si="117">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -25569,7 +25585,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5:K20" si="7">J5</f>
+        <f t="shared" ref="K5" si="7">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -25581,7 +25597,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5:O20" si="9">N5</f>
+        <f t="shared" ref="O5" si="9">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -25596,7 +25612,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5:S20" si="11">R5</f>
+        <f t="shared" ref="S5" si="11">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -25611,7 +25627,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5:W20" si="13">V5</f>
+        <f t="shared" ref="W5" si="13">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -25626,7 +25642,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5:AA20" si="15">Z5</f>
+        <f t="shared" ref="AA5" si="15">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -26036,7 +26052,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10:K25" si="17">J10</f>
+        <f t="shared" ref="K10" si="17">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -26048,7 +26064,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10:O25" si="18">N10</f>
+        <f t="shared" ref="O10" si="18">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -26060,7 +26076,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10:S25" si="19">R10</f>
+        <f t="shared" ref="S10" si="19">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -26075,7 +26091,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10:W25" si="20">V10</f>
+        <f t="shared" ref="W10" si="20">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -26087,7 +26103,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10:AA25" si="21">Z10</f>
+        <f t="shared" ref="AA10" si="21">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -28457,7 +28473,7 @@
         <v>85</v>
       </c>
       <c r="M36" s="16">
-        <f t="shared" ref="M36:M49" si="35">L36</f>
+        <f t="shared" ref="M36:M37" si="35">L36</f>
         <v>85</v>
       </c>
       <c r="N36" s="11">
@@ -28472,7 +28488,7 @@
         <v>100</v>
       </c>
       <c r="Q36" s="16">
-        <f t="shared" ref="Q36:Q49" si="36">P36</f>
+        <f t="shared" ref="Q36:Q37" si="36">P36</f>
         <v>100</v>
       </c>
       <c r="R36" s="11">
@@ -28487,7 +28503,7 @@
         <v>90</v>
       </c>
       <c r="U36" s="16">
-        <f t="shared" ref="U36:U49" si="37">T36</f>
+        <f t="shared" ref="U36:U37" si="37">T36</f>
         <v>90</v>
       </c>
       <c r="V36" s="11">
@@ -28502,7 +28518,7 @@
         <v>85</v>
       </c>
       <c r="Y36" s="16">
-        <f t="shared" ref="Y36:Y49" si="38">X36</f>
+        <f t="shared" ref="Y36:Y37" si="38">X36</f>
         <v>85</v>
       </c>
       <c r="Z36" s="11">
@@ -28517,7 +28533,7 @@
         <v>90</v>
       </c>
       <c r="AC36" s="16">
-        <f t="shared" ref="AC36:AC49" si="39">AB36</f>
+        <f t="shared" ref="AC36:AC37" si="39">AB36</f>
         <v>90</v>
       </c>
     </row>
@@ -28551,11 +28567,11 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37:K44" si="41">J37</f>
+        <f t="shared" ref="K37" si="41">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37:L44" si="42">K37</f>
+        <f t="shared" ref="L37" si="42">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
@@ -28563,11 +28579,11 @@
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37:O44" si="43">N37</f>
+        <f t="shared" ref="O37" si="43">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37:P44" si="44">O37</f>
+        <f t="shared" ref="P37" si="44">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
@@ -28578,11 +28594,11 @@
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37:S44" si="45">R37</f>
+        <f t="shared" ref="S37" si="45">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37:T44" si="46">S37</f>
+        <f t="shared" ref="T37" si="46">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
@@ -28590,11 +28606,11 @@
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37:W44" si="47">V37</f>
+        <f t="shared" ref="W37" si="47">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37:X44" si="48">W37</f>
+        <f t="shared" ref="X37" si="48">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
@@ -28602,11 +28618,11 @@
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37:AA44" si="49">Z37</f>
+        <f t="shared" ref="AA37" si="49">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37:AB44" si="50">AA37</f>
+        <f t="shared" ref="AB37" si="50">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
@@ -28756,7 +28772,7 @@
         <v>85</v>
       </c>
       <c r="M39" s="16">
-        <f t="shared" ref="M39:M52" si="51">L39</f>
+        <f t="shared" ref="M39:M40" si="51">L39</f>
         <v>85</v>
       </c>
       <c r="O39" s="12">
@@ -28768,7 +28784,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="16">
-        <f t="shared" ref="Q39:Q52" si="52">P39</f>
+        <f t="shared" ref="Q39:Q40" si="52">P39</f>
         <v>0</v>
       </c>
       <c r="R39" s="11">
@@ -28783,7 +28799,7 @@
         <v>90</v>
       </c>
       <c r="U39" s="16">
-        <f t="shared" ref="U39:U52" si="53">T39</f>
+        <f t="shared" ref="U39:U40" si="53">T39</f>
         <v>90</v>
       </c>
       <c r="W39" s="12">
@@ -28795,7 +28811,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="16">
-        <f t="shared" ref="Y39:Y52" si="54">X39</f>
+        <f t="shared" ref="Y39:Y40" si="54">X39</f>
         <v>0</v>
       </c>
       <c r="AA39" s="12">
@@ -28807,7 +28823,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="16">
-        <f t="shared" ref="AC39:AC52" si="55">AB39</f>
+        <f t="shared" ref="AC39:AC40" si="55">AB39</f>
         <v>0</v>
       </c>
     </row>
@@ -28838,11 +28854,11 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40:K47" si="56">J40</f>
+        <f t="shared" ref="K40" si="56">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40:L47" si="57">K40</f>
+        <f t="shared" ref="L40" si="57">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
@@ -28853,11 +28869,11 @@
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40:O47" si="58">N40</f>
+        <f t="shared" ref="O40" si="58">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40:P47" si="59">O40</f>
+        <f t="shared" ref="P40" si="59">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
@@ -28868,11 +28884,11 @@
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40:S47" si="60">R40</f>
+        <f t="shared" ref="S40" si="60">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40:T47" si="61">S40</f>
+        <f t="shared" ref="T40" si="61">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
@@ -28883,11 +28899,11 @@
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40:W47" si="62">V40</f>
+        <f t="shared" ref="W40" si="62">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40:X47" si="63">W40</f>
+        <f t="shared" ref="X40" si="63">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
@@ -28898,11 +28914,11 @@
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40:AA47" si="64">Z40</f>
+        <f t="shared" ref="AA40" si="64">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40:AB47" si="65">AA40</f>
+        <f t="shared" ref="AB40" si="65">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
@@ -29160,7 +29176,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M56" si="66">L43</f>
+        <f t="shared" ref="M43:M44" si="66">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -29175,7 +29191,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q56" si="67">P43</f>
+        <f t="shared" ref="Q43:Q44" si="67">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -29190,7 +29206,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U56" si="68">T43</f>
+        <f t="shared" ref="U43:U44" si="68">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -29205,7 +29221,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y56" si="69">X43</f>
+        <f t="shared" ref="Y43:Y44" si="69">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -29220,7 +29236,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC56" si="70">AB43</f>
+        <f t="shared" ref="AC43:AC44" si="70">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -29251,11 +29267,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44:K51" si="71">J44</f>
+        <f t="shared" ref="K44" si="71">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44:L51" si="72">K44</f>
+        <f t="shared" ref="L44" si="72">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -29266,11 +29282,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44:O51" si="73">N44</f>
+        <f t="shared" ref="O44" si="73">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44:P51" si="74">O44</f>
+        <f t="shared" ref="P44" si="74">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -29281,11 +29297,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44:S51" si="75">R44</f>
+        <f t="shared" ref="S44" si="75">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44:T51" si="76">S44</f>
+        <f t="shared" ref="T44" si="76">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -29293,11 +29309,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44:W51" si="77">V44</f>
+        <f t="shared" ref="W44" si="77">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44:X51" si="78">W44</f>
+        <f t="shared" ref="X44" si="78">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -29308,11 +29324,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44:AA51" si="79">Z44</f>
+        <f t="shared" ref="AA44" si="79">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44:AB51" si="80">AA44</f>
+        <f t="shared" ref="AB44" si="80">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -29357,7 +29373,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="15">
-        <f t="shared" ref="L45:L55" si="82">K45*$D45</f>
+        <f t="shared" ref="L45" si="82">K45*$D45</f>
         <v>0</v>
       </c>
       <c r="M45" s="16">
@@ -29372,7 +29388,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" ref="P45:P55" si="83">O45*$D45</f>
+        <f t="shared" ref="P45" si="83">O45*$D45</f>
         <v>3.7499999999999999E-3</v>
       </c>
       <c r="Q45" s="16">
@@ -29387,7 +29403,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="T45" s="15">
-        <f t="shared" ref="T45:T55" si="84">S45*$D45</f>
+        <f t="shared" ref="T45" si="84">S45*$D45</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="U45" s="16">
@@ -29399,7 +29415,7 @@
         <v>0</v>
       </c>
       <c r="X45" s="15">
-        <f t="shared" ref="X45:X55" si="85">W45*$D45</f>
+        <f t="shared" ref="X45" si="85">W45*$D45</f>
         <v>0</v>
       </c>
       <c r="Y45" s="16">
@@ -29414,7 +29430,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AB45" s="15">
-        <f t="shared" ref="AB45:AB55" si="86">AA45*$D45</f>
+        <f t="shared" ref="AB45" si="86">AA45*$D45</f>
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="AC45" s="16">
@@ -29564,7 +29580,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47:M60" si="87">L47</f>
+        <f t="shared" ref="M47" si="87">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -29579,7 +29595,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47:Q60" si="88">P47</f>
+        <f t="shared" ref="Q47" si="88">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -29594,7 +29610,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47:U60" si="89">T47</f>
+        <f t="shared" ref="U47" si="89">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -29606,7 +29622,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47:Y60" si="90">X47</f>
+        <f t="shared" ref="Y47" si="90">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -29621,7 +29637,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47:AC60" si="91">AB47</f>
+        <f t="shared" ref="AC47" si="91">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -29665,7 +29681,7 @@
         <v>2</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" ref="L48:L58" si="92">K48*$D48</f>
+        <f t="shared" ref="L48" si="92">K48*$D48</f>
         <v>1.5</v>
       </c>
       <c r="M48" s="16">
@@ -29677,7 +29693,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="15">
-        <f t="shared" ref="P48:P58" si="93">O48*$D48</f>
+        <f t="shared" ref="P48" si="93">O48*$D48</f>
         <v>0</v>
       </c>
       <c r="Q48" s="16">
@@ -29692,7 +29708,7 @@
         <v>1</v>
       </c>
       <c r="T48" s="15">
-        <f t="shared" ref="T48:T58" si="94">S48*$D48</f>
+        <f t="shared" ref="T48" si="94">S48*$D48</f>
         <v>0.75</v>
       </c>
       <c r="U48" s="16">
@@ -29707,7 +29723,7 @@
         <v>2</v>
       </c>
       <c r="X48" s="15">
-        <f t="shared" ref="X48:X58" si="95">W48*$D48</f>
+        <f t="shared" ref="X48" si="95">W48*$D48</f>
         <v>1.5</v>
       </c>
       <c r="Y48" s="16">
@@ -29722,7 +29738,7 @@
         <v>1</v>
       </c>
       <c r="AB48" s="15">
-        <f t="shared" ref="AB48:AB58" si="96">AA48*$D48</f>
+        <f t="shared" ref="AB48" si="96">AA48*$D48</f>
         <v>0.75</v>
       </c>
       <c r="AC48" s="16">
@@ -29875,7 +29891,7 @@
         <v>2</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" ref="L50:L60" si="97">K50*$D50</f>
+        <f t="shared" ref="L50:L55" si="97">K50*$D50</f>
         <v>1.5</v>
       </c>
       <c r="M50" s="16">
@@ -29887,7 +29903,7 @@
         <v>1.5</v>
       </c>
       <c r="P50" s="15">
-        <f t="shared" ref="P50:P60" si="98">O50*$D50</f>
+        <f t="shared" ref="P50:P55" si="98">O50*$D50</f>
         <v>1.125</v>
       </c>
       <c r="Q50" s="16">
@@ -29902,7 +29918,7 @@
         <v>1.5</v>
       </c>
       <c r="T50" s="15">
-        <f t="shared" ref="T50:T60" si="99">S50*$D50</f>
+        <f t="shared" ref="T50:T55" si="99">S50*$D50</f>
         <v>1.125</v>
       </c>
       <c r="U50" s="16">
@@ -29917,7 +29933,7 @@
         <v>2</v>
       </c>
       <c r="X50" s="15">
-        <f t="shared" ref="X50:X60" si="100">W50*$D50</f>
+        <f t="shared" ref="X50:X55" si="100">W50*$D50</f>
         <v>1.5</v>
       </c>
       <c r="Y50" s="16">
@@ -29932,7 +29948,7 @@
         <v>1.5</v>
       </c>
       <c r="AB50" s="15">
-        <f t="shared" ref="AB50:AB60" si="101">AA50*$D50</f>
+        <f t="shared" ref="AB50:AB55" si="101">AA50*$D50</f>
         <v>1.125</v>
       </c>
       <c r="AC50" s="16">
@@ -30182,7 +30198,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" ref="K53:K93" si="103">J53</f>
+        <f t="shared" ref="K53:K60" si="103">J53</f>
         <v>0</v>
       </c>
       <c r="L53" s="15">
@@ -30194,7 +30210,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="12">
-        <f t="shared" ref="O53:O93" si="104">N53</f>
+        <f t="shared" ref="O53:O60" si="104">N53</f>
         <v>0</v>
       </c>
       <c r="P53" s="15">
@@ -30209,7 +30225,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="12">
-        <f t="shared" ref="S53:S93" si="105">R53</f>
+        <f t="shared" ref="S53:S60" si="105">R53</f>
         <v>1</v>
       </c>
       <c r="T53" s="15">
@@ -30224,7 +30240,7 @@
         <v>1.2</v>
       </c>
       <c r="W53" s="12">
-        <f t="shared" ref="W53:W93" si="106">V53</f>
+        <f t="shared" ref="W53:W60" si="106">V53</f>
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
@@ -30239,7 +30255,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53" s="12">
-        <f t="shared" ref="AA53:AA93" si="107">Z53</f>
+        <f t="shared" ref="AA53:AA60" si="107">Z53</f>
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
@@ -31049,7 +31065,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" ref="K62:K93" si="113">J62</f>
+        <f t="shared" ref="K62:K79" si="113">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="15">
@@ -31061,7 +31077,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="12">
-        <f t="shared" ref="O62:O93" si="114">N62</f>
+        <f t="shared" ref="O62:O79" si="114">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="15">
@@ -31076,7 +31092,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="12">
-        <f t="shared" ref="S62:S93" si="115">R62</f>
+        <f t="shared" ref="S62:S79" si="115">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="15">
@@ -31091,7 +31107,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="12">
-        <f t="shared" ref="W62:W93" si="116">V62</f>
+        <f t="shared" ref="W62:W79" si="116">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="15">
@@ -31106,7 +31122,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="12">
-        <f t="shared" ref="AA62:AA93" si="117">Z62</f>
+        <f t="shared" ref="AA62:AA79" si="117">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="15">
@@ -31428,7 +31444,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="16">
-        <f t="shared" ref="M66:M93" si="119">L66</f>
+        <f t="shared" ref="M66:M85" si="119">L66</f>
         <v>0</v>
       </c>
       <c r="O66" s="12">
@@ -31440,7 +31456,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="16">
-        <f t="shared" ref="Q66:Q93" si="120">P66</f>
+        <f t="shared" ref="Q66:Q85" si="120">P66</f>
         <v>0</v>
       </c>
       <c r="S66" s="12">
@@ -31452,7 +31468,7 @@
         <v>0</v>
       </c>
       <c r="U66" s="16">
-        <f t="shared" ref="U66:U93" si="121">T66</f>
+        <f t="shared" ref="U66:U85" si="121">T66</f>
         <v>0</v>
       </c>
       <c r="W66" s="12">
@@ -31464,7 +31480,7 @@
         <v>0</v>
       </c>
       <c r="Y66" s="16">
-        <f t="shared" ref="Y66:Y93" si="122">X66</f>
+        <f t="shared" ref="Y66:Y85" si="122">X66</f>
         <v>0</v>
       </c>
       <c r="AA66" s="12">
@@ -31476,7 +31492,7 @@
         <v>0</v>
       </c>
       <c r="AC66" s="16">
-        <f t="shared" ref="AC66:AC93" si="123">AB66</f>
+        <f t="shared" ref="AC66:AC85" si="123">AB66</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected expected values in wind, mech remove and mech add
</commit_message>
<xml_diff>
--- a/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
+++ b/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -2705,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD67"/>
+    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C7" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7539,8 +7539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7973,7 +7973,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5" si="8">J5</f>
+        <f t="shared" ref="K5:K15" si="8">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -7985,7 +7985,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5" si="10">N5</f>
+        <f t="shared" ref="O5:O15" si="10">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -8000,7 +8000,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5" si="12">R5</f>
+        <f t="shared" ref="S5:S15" si="12">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -8015,7 +8015,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5" si="14">V5</f>
+        <f t="shared" ref="W5:W15" si="14">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -8030,7 +8030,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5" si="16">Z5</f>
+        <f t="shared" ref="AA5:AA15" si="16">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -8247,7 +8247,7 @@
         <v>291</v>
       </c>
       <c r="C8" s="4">
-        <v>1.25</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -8304,15 +8304,15 @@
       </c>
       <c r="W8" s="12">
         <f>$C8*V8</f>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="X8" s="15">
         <f t="shared" si="15"/>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="Y8" s="16">
         <f t="shared" si="4"/>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="AA8" s="12">
         <f>$C8*Z8</f>
@@ -8440,7 +8440,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10" si="18">J10</f>
+        <f t="shared" ref="K10:K20" si="18">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -8452,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10" si="19">N10</f>
+        <f t="shared" ref="O10:O20" si="19">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -8464,7 +8464,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10" si="20">R10</f>
+        <f t="shared" ref="S10:S20" si="20">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -8479,7 +8479,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10" si="21">V10</f>
+        <f t="shared" ref="W10:W20" si="21">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -8491,7 +8491,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10" si="22">Z10</f>
+        <f t="shared" ref="AA10:AA20" si="22">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -8705,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" ref="K13:K15" si="23">J13</f>
+        <f t="shared" ref="K13:K23" si="23">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
@@ -8717,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" ref="O13:O15" si="24">N13</f>
+        <f t="shared" ref="O13:O23" si="24">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
@@ -8732,7 +8732,7 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" ref="S13:S15" si="25">R13</f>
+        <f t="shared" ref="S13:S23" si="25">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="15">
@@ -8747,7 +8747,7 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="12">
-        <f t="shared" ref="W13:W15" si="26">V13</f>
+        <f t="shared" ref="W13:W23" si="26">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="15">
@@ -8762,7 +8762,7 @@
         <v>1</v>
       </c>
       <c r="AA13" s="12">
-        <f t="shared" ref="AA13:AA15" si="27">Z13</f>
+        <f t="shared" ref="AA13:AA23" si="27">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="15">
@@ -10640,7 +10640,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34" si="36">L34</f>
+        <f t="shared" ref="M34:M47" si="36">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -10655,7 +10655,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34" si="37">P34</f>
+        <f t="shared" ref="Q34:Q47" si="37">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -10670,7 +10670,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34" si="38">T34</f>
+        <f t="shared" ref="U34:U47" si="38">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -10685,7 +10685,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34" si="39">X34</f>
+        <f t="shared" ref="Y34:Y47" si="39">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -10700,7 +10700,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34" si="40">AB34</f>
+        <f t="shared" ref="AC34:AC47" si="40">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -10949,66 +10949,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37" si="43">J37</f>
+        <f t="shared" ref="K37:K44" si="43">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37" si="44">K37</f>
+        <f t="shared" ref="L37:L44" si="44">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37" si="45">L37</f>
+        <f t="shared" ref="M37:M50" si="45">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37" si="46">N37</f>
+        <f t="shared" ref="O37:O44" si="46">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37" si="47">O37</f>
+        <f t="shared" ref="P37:P44" si="47">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37" si="48">P37</f>
+        <f t="shared" ref="Q37:Q50" si="48">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37" si="49">R37</f>
+        <f t="shared" ref="S37:S44" si="49">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37" si="50">S37</f>
+        <f t="shared" ref="T37:T44" si="50">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37" si="51">T37</f>
+        <f t="shared" ref="U37:U50" si="51">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37" si="52">V37</f>
+        <f t="shared" ref="W37:W44" si="52">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37" si="53">W37</f>
+        <f t="shared" ref="X37:X44" si="53">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37" si="54">X37</f>
+        <f t="shared" ref="Y37:Y50" si="54">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37" si="55">Z37</f>
+        <f t="shared" ref="AA37:AA44" si="55">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37" si="56">AA37</f>
+        <f t="shared" ref="AB37:AB44" si="56">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37" si="57">AB37</f>
+        <f t="shared" ref="AC37:AC50" si="57">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -11236,75 +11236,75 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40" si="58">J40</f>
+        <f t="shared" ref="K40:K47" si="58">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40" si="59">K40</f>
+        <f t="shared" ref="L40:L47" si="59">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" ref="M40" si="60">L40</f>
+        <f t="shared" ref="M40:M53" si="60">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="11">
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40" si="61">N40</f>
+        <f t="shared" ref="O40:O47" si="61">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40" si="62">O40</f>
+        <f t="shared" ref="P40:P47" si="62">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
-        <f t="shared" ref="Q40" si="63">P40</f>
+        <f t="shared" ref="Q40:Q53" si="63">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="11">
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40" si="64">R40</f>
+        <f t="shared" ref="S40:S47" si="64">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40" si="65">S40</f>
+        <f t="shared" ref="T40:T47" si="65">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" ref="U40" si="66">T40</f>
+        <f t="shared" ref="U40:U53" si="66">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="11">
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40" si="67">V40</f>
+        <f t="shared" ref="W40:W47" si="67">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40" si="68">W40</f>
+        <f t="shared" ref="X40:X47" si="68">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
-        <f t="shared" ref="Y40" si="69">X40</f>
+        <f t="shared" ref="Y40:Y53" si="69">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="11">
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40" si="70">Z40</f>
+        <f t="shared" ref="AA40:AA47" si="70">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40" si="71">AA40</f>
+        <f t="shared" ref="AB40:AB47" si="71">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
-        <f t="shared" ref="AC40" si="72">AB40</f>
+        <f t="shared" ref="AC40:AC53" si="72">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -11558,7 +11558,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M44" si="73">L43</f>
+        <f t="shared" ref="M43:M56" si="73">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -11573,7 +11573,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q44" si="74">P43</f>
+        <f t="shared" ref="Q43:Q56" si="74">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -11588,7 +11588,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U44" si="75">T43</f>
+        <f t="shared" ref="U43:U56" si="75">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -11603,7 +11603,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y44" si="76">X43</f>
+        <f t="shared" ref="Y43:Y56" si="76">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -11618,7 +11618,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC44" si="77">AB43</f>
+        <f t="shared" ref="AC43:AC56" si="77">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -11649,11 +11649,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44" si="78">J44</f>
+        <f t="shared" ref="K44:K51" si="78">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44" si="79">K44</f>
+        <f t="shared" ref="L44:L51" si="79">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -11664,11 +11664,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44" si="80">N44</f>
+        <f t="shared" ref="O44:O51" si="80">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44" si="81">O44</f>
+        <f t="shared" ref="P44:P51" si="81">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -11679,11 +11679,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44" si="82">R44</f>
+        <f t="shared" ref="S44:S51" si="82">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44" si="83">S44</f>
+        <f t="shared" ref="T44:T51" si="83">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -11691,11 +11691,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44" si="84">V44</f>
+        <f t="shared" ref="W44:W51" si="84">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44" si="85">W44</f>
+        <f t="shared" ref="X44:X51" si="85">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -11706,11 +11706,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44" si="86">Z44</f>
+        <f t="shared" ref="AA44:AA51" si="86">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44" si="87">AA44</f>
+        <f t="shared" ref="AB44:AB51" si="87">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -11962,7 +11962,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47" si="88">L47</f>
+        <f t="shared" ref="M47:M60" si="88">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -11977,7 +11977,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47" si="89">P47</f>
+        <f t="shared" ref="Q47:Q60" si="89">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -11992,7 +11992,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47" si="90">T47</f>
+        <f t="shared" ref="U47:U60" si="90">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -12004,7 +12004,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47" si="91">X47</f>
+        <f t="shared" ref="Y47:Y60" si="91">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -12019,7 +12019,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47" si="92">AB47</f>
+        <f t="shared" ref="AC47:AC60" si="92">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -12580,7 +12580,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" ref="K53:K60" si="100">J53</f>
+        <f t="shared" ref="K53:K93" si="100">J53</f>
         <v>0</v>
       </c>
       <c r="L53" s="15">
@@ -12592,7 +12592,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="12">
-        <f t="shared" ref="O53:O60" si="101">N53</f>
+        <f t="shared" ref="O53:O93" si="101">N53</f>
         <v>0</v>
       </c>
       <c r="P53" s="15">
@@ -12607,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="12">
-        <f t="shared" ref="S53:S60" si="102">R53</f>
+        <f t="shared" ref="S53:S93" si="102">R53</f>
         <v>1</v>
       </c>
       <c r="T53" s="15">
@@ -12622,7 +12622,7 @@
         <v>1.2</v>
       </c>
       <c r="W53" s="12">
-        <f t="shared" ref="W53:W60" si="103">V53</f>
+        <f t="shared" ref="W53:W93" si="103">V53</f>
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
@@ -12637,7 +12637,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53" s="12">
-        <f t="shared" ref="AA53:AA60" si="104">Z53</f>
+        <f t="shared" ref="AA53:AA93" si="104">Z53</f>
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
@@ -13447,7 +13447,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="40">
-        <f t="shared" ref="K62:K79" si="110">J62</f>
+        <f t="shared" ref="K62:K93" si="110">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="41">
@@ -13459,7 +13459,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="40">
-        <f t="shared" ref="O62:O79" si="111">N62</f>
+        <f t="shared" ref="O62:O93" si="111">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="41">
@@ -13474,7 +13474,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="40">
-        <f t="shared" ref="S62:S79" si="112">R62</f>
+        <f t="shared" ref="S62:S93" si="112">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="41">
@@ -13489,7 +13489,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="40">
-        <f t="shared" ref="W62:W79" si="113">V62</f>
+        <f t="shared" ref="W62:W93" si="113">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="41">
@@ -13504,7 +13504,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="40">
-        <f t="shared" ref="AA62:AA79" si="114">Z62</f>
+        <f t="shared" ref="AA62:AA93" si="114">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="41">
@@ -35844,15 +35844,15 @@
       </c>
       <c r="AQ8">
         <f>'2_MechAdd_LowSeverity'!W8</f>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="AR8">
         <f>'2_MechAdd_LowSeverity'!X8</f>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="AS8">
         <f>'2_MechAdd_LowSeverity'!Y8</f>
-        <v>9.375</v>
+        <v>8.25</v>
       </c>
       <c r="AT8">
         <f>'2_MechAdd_ModSeverity'!W8</f>

</xml_diff>

<commit_message>
Changed specs and expected values for fire and mech remove.
</commit_message>
<xml_diff>
--- a/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
+++ b/specifications/2_MechAdd/ScriptRules_MechAdd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -2705,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C7" sqref="C1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,7 +2757,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>93</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>88</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>90</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>89</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>91</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>92</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>83</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>85</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>84</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>86</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>87</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>94</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>96</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>95</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>97</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>98</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>69</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>70</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>71</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>74</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>72</v>
       </c>
@@ -3052,7 +3052,7 @@
       <c r="G22" s="22"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>73</v>
       </c>
@@ -3063,7 +3063,7 @@
       <c r="G23" s="22"/>
       <c r="J23" s="22"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>75</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>76</v>
       </c>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>77</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>78</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>79</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>80</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>81</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>82</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>67</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>68</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>133</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="J34" s="22"/>
       <c r="K34" s="23"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>134</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>135</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="K36" s="23"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>136</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="H37" s="23"/>
       <c r="K37" s="23"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>137</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>138</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="K39" s="23"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>111</v>
       </c>
@@ -3308,7 +3308,7 @@
       <c r="J40" s="22"/>
       <c r="K40" s="23"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>112</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>113</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>114</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="K43" s="23"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>115</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="J44" s="22"/>
       <c r="K44" s="23"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>116</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>117</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>118</v>
       </c>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="K47" s="23"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>139</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>140</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>144</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>145</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>146</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>206</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>207</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>208</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>209</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>210</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>211</v>
       </c>
@@ -7539,8 +7539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView topLeftCell="A62" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7973,7 +7973,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5:K15" si="8">J5</f>
+        <f t="shared" ref="K5" si="8">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
@@ -7985,7 +7985,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5:O15" si="10">N5</f>
+        <f t="shared" ref="O5" si="10">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -8000,7 +8000,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5:S15" si="12">R5</f>
+        <f t="shared" ref="S5" si="12">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
@@ -8015,7 +8015,7 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5:W15" si="14">V5</f>
+        <f t="shared" ref="W5" si="14">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
@@ -8030,7 +8030,7 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5:AA15" si="16">Z5</f>
+        <f t="shared" ref="AA5" si="16">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
@@ -8440,7 +8440,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10:K20" si="18">J10</f>
+        <f t="shared" ref="K10" si="18">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
@@ -8452,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10:O20" si="19">N10</f>
+        <f t="shared" ref="O10" si="19">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
@@ -8464,7 +8464,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10:S20" si="20">R10</f>
+        <f t="shared" ref="S10" si="20">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
@@ -8479,7 +8479,7 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10:W20" si="21">V10</f>
+        <f t="shared" ref="W10" si="21">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
@@ -8491,7 +8491,7 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10:AA20" si="22">Z10</f>
+        <f t="shared" ref="AA10" si="22">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
@@ -8705,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" ref="K13:K23" si="23">J13</f>
+        <f t="shared" ref="K13:K15" si="23">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
@@ -8717,7 +8717,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" ref="O13:O23" si="24">N13</f>
+        <f t="shared" ref="O13:O15" si="24">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
@@ -8732,7 +8732,7 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" ref="S13:S23" si="25">R13</f>
+        <f t="shared" ref="S13:S15" si="25">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="15">
@@ -8747,7 +8747,7 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="12">
-        <f t="shared" ref="W13:W23" si="26">V13</f>
+        <f t="shared" ref="W13:W15" si="26">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="15">
@@ -8762,7 +8762,7 @@
         <v>1</v>
       </c>
       <c r="AA13" s="12">
-        <f t="shared" ref="AA13:AA23" si="27">Z13</f>
+        <f t="shared" ref="AA13:AA15" si="27">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="15">
@@ -10640,7 +10640,7 @@
         <v>5</v>
       </c>
       <c r="M34" s="16">
-        <f t="shared" ref="M34:M47" si="36">L34</f>
+        <f t="shared" ref="M34" si="36">L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="11">
@@ -10655,7 +10655,7 @@
         <v>3</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" ref="Q34:Q47" si="37">P34</f>
+        <f t="shared" ref="Q34" si="37">P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="11">
@@ -10670,7 +10670,7 @@
         <v>5</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" ref="U34:U47" si="38">T34</f>
+        <f t="shared" ref="U34" si="38">T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="11">
@@ -10685,7 +10685,7 @@
         <v>6</v>
       </c>
       <c r="Y34" s="16">
-        <f t="shared" ref="Y34:Y47" si="39">X34</f>
+        <f t="shared" ref="Y34" si="39">X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="11">
@@ -10700,7 +10700,7 @@
         <v>5</v>
       </c>
       <c r="AC34" s="16">
-        <f t="shared" ref="AC34:AC47" si="40">AB34</f>
+        <f t="shared" ref="AC34" si="40">AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -10949,66 +10949,66 @@
         <v>2</v>
       </c>
       <c r="K37" s="12">
-        <f t="shared" ref="K37:K44" si="43">J37</f>
+        <f t="shared" ref="K37" si="43">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" ref="L37:L44" si="44">K37</f>
+        <f t="shared" ref="L37" si="44">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="16">
-        <f t="shared" ref="M37:M50" si="45">L37</f>
+        <f t="shared" ref="M37" si="45">L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="12">
-        <f t="shared" ref="O37:O44" si="46">N37</f>
+        <f t="shared" ref="O37" si="46">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" ref="P37:P44" si="47">O37</f>
+        <f t="shared" ref="P37" si="47">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" ref="Q37:Q50" si="48">P37</f>
+        <f t="shared" ref="Q37" si="48">P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="11">
         <v>1</v>
       </c>
       <c r="S37" s="12">
-        <f t="shared" ref="S37:S44" si="49">R37</f>
+        <f t="shared" ref="S37" si="49">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="15">
-        <f t="shared" ref="T37:T44" si="50">S37</f>
+        <f t="shared" ref="T37" si="50">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" ref="U37:U50" si="51">T37</f>
+        <f t="shared" ref="U37" si="51">T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="12">
-        <f t="shared" ref="W37:W44" si="52">V37</f>
+        <f t="shared" ref="W37" si="52">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="15">
-        <f t="shared" ref="X37:X44" si="53">W37</f>
+        <f t="shared" ref="X37" si="53">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="16">
-        <f t="shared" ref="Y37:Y50" si="54">X37</f>
+        <f t="shared" ref="Y37" si="54">X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="12">
-        <f t="shared" ref="AA37:AA44" si="55">Z37</f>
+        <f t="shared" ref="AA37" si="55">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="15">
-        <f t="shared" ref="AB37:AB44" si="56">AA37</f>
+        <f t="shared" ref="AB37" si="56">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="16">
-        <f t="shared" ref="AC37:AC50" si="57">AB37</f>
+        <f t="shared" ref="AC37" si="57">AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -11236,75 +11236,75 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="12">
-        <f t="shared" ref="K40:K47" si="58">J40</f>
+        <f t="shared" ref="K40" si="58">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" ref="L40:L47" si="59">K40</f>
+        <f t="shared" ref="L40" si="59">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="16">
-        <f t="shared" ref="M40:M53" si="60">L40</f>
+        <f t="shared" ref="M40" si="60">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="11">
         <v>2</v>
       </c>
       <c r="O40" s="12">
-        <f t="shared" ref="O40:O47" si="61">N40</f>
+        <f t="shared" ref="O40" si="61">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" ref="P40:P47" si="62">O40</f>
+        <f t="shared" ref="P40" si="62">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="16">
-        <f t="shared" ref="Q40:Q53" si="63">P40</f>
+        <f t="shared" ref="Q40" si="63">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="11">
         <v>1</v>
       </c>
       <c r="S40" s="12">
-        <f t="shared" ref="S40:S47" si="64">R40</f>
+        <f t="shared" ref="S40" si="64">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="15">
-        <f t="shared" ref="T40:T47" si="65">S40</f>
+        <f t="shared" ref="T40" si="65">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" ref="U40:U53" si="66">T40</f>
+        <f t="shared" ref="U40" si="66">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="11">
         <v>2.5</v>
       </c>
       <c r="W40" s="12">
-        <f t="shared" ref="W40:W47" si="67">V40</f>
+        <f t="shared" ref="W40" si="67">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="15">
-        <f t="shared" ref="X40:X47" si="68">W40</f>
+        <f t="shared" ref="X40" si="68">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="16">
-        <f t="shared" ref="Y40:Y53" si="69">X40</f>
+        <f t="shared" ref="Y40" si="69">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="11">
         <v>2</v>
       </c>
       <c r="AA40" s="12">
-        <f t="shared" ref="AA40:AA47" si="70">Z40</f>
+        <f t="shared" ref="AA40" si="70">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="15">
-        <f t="shared" ref="AB40:AB47" si="71">AA40</f>
+        <f t="shared" ref="AB40" si="71">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="16">
-        <f t="shared" ref="AC40:AC53" si="72">AB40</f>
+        <f t="shared" ref="AC40" si="72">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -11558,7 +11558,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" ref="M43:M56" si="73">L43</f>
+        <f t="shared" ref="M43:M44" si="73">L43</f>
         <v>0</v>
       </c>
       <c r="N43" s="11">
@@ -11573,7 +11573,7 @@
         <v>85</v>
       </c>
       <c r="Q43" s="16">
-        <f t="shared" ref="Q43:Q56" si="74">P43</f>
+        <f t="shared" ref="Q43:Q44" si="74">P43</f>
         <v>85</v>
       </c>
       <c r="R43" s="11">
@@ -11588,7 +11588,7 @@
         <v>90</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" ref="U43:U56" si="75">T43</f>
+        <f t="shared" ref="U43:U44" si="75">T43</f>
         <v>90</v>
       </c>
       <c r="V43" s="11">
@@ -11603,7 +11603,7 @@
         <v>80</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" ref="Y43:Y56" si="76">X43</f>
+        <f t="shared" ref="Y43:Y44" si="76">X43</f>
         <v>80</v>
       </c>
       <c r="Z43" s="11">
@@ -11618,7 +11618,7 @@
         <v>60</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" ref="AC43:AC56" si="77">AB43</f>
+        <f t="shared" ref="AC43:AC44" si="77">AB43</f>
         <v>60</v>
       </c>
     </row>
@@ -11649,11 +11649,11 @@
         <v>0.9</v>
       </c>
       <c r="K44" s="12">
-        <f t="shared" ref="K44:K51" si="78">J44</f>
+        <f t="shared" ref="K44" si="78">J44</f>
         <v>0</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" ref="L44:L51" si="79">K44</f>
+        <f t="shared" ref="L44" si="79">K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="16">
@@ -11664,11 +11664,11 @@
         <v>1</v>
       </c>
       <c r="O44" s="12">
-        <f t="shared" ref="O44:O51" si="80">N44</f>
+        <f t="shared" ref="O44" si="80">N44</f>
         <v>1</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" ref="P44:P51" si="81">O44</f>
+        <f t="shared" ref="P44" si="81">O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="16">
@@ -11679,11 +11679,11 @@
         <v>0.5</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44:S51" si="82">R44</f>
+        <f t="shared" ref="S44" si="82">R44</f>
         <v>0.5</v>
       </c>
       <c r="T44" s="15">
-        <f t="shared" ref="T44:T51" si="83">S44</f>
+        <f t="shared" ref="T44" si="83">S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="16">
@@ -11691,11 +11691,11 @@
         <v>0.5</v>
       </c>
       <c r="W44" s="12">
-        <f t="shared" ref="W44:W51" si="84">V44</f>
+        <f t="shared" ref="W44" si="84">V44</f>
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <f t="shared" ref="X44:X51" si="85">W44</f>
+        <f t="shared" ref="X44" si="85">W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="16">
@@ -11706,11 +11706,11 @@
         <v>1</v>
       </c>
       <c r="AA44" s="12">
-        <f t="shared" ref="AA44:AA51" si="86">Z44</f>
+        <f t="shared" ref="AA44" si="86">Z44</f>
         <v>1</v>
       </c>
       <c r="AB44" s="15">
-        <f t="shared" ref="AB44:AB51" si="87">AA44</f>
+        <f t="shared" ref="AB44" si="87">AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="16">
@@ -11962,7 +11962,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="16">
-        <f t="shared" ref="M47:M60" si="88">L47</f>
+        <f t="shared" ref="M47" si="88">L47</f>
         <v>0</v>
       </c>
       <c r="N47" s="11">
@@ -11977,7 +11977,7 @@
         <v>70</v>
       </c>
       <c r="Q47" s="16">
-        <f t="shared" ref="Q47:Q60" si="89">P47</f>
+        <f t="shared" ref="Q47" si="89">P47</f>
         <v>70</v>
       </c>
       <c r="R47" s="11">
@@ -11992,7 +11992,7 @@
         <v>90</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" ref="U47:U60" si="90">T47</f>
+        <f t="shared" ref="U47" si="90">T47</f>
         <v>90</v>
       </c>
       <c r="W47" s="12">
@@ -12004,7 +12004,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="16">
-        <f t="shared" ref="Y47:Y60" si="91">X47</f>
+        <f t="shared" ref="Y47" si="91">X47</f>
         <v>0</v>
       </c>
       <c r="Z47" s="11">
@@ -12019,7 +12019,7 @@
         <v>60</v>
       </c>
       <c r="AC47" s="16">
-        <f t="shared" ref="AC47:AC60" si="92">AB47</f>
+        <f t="shared" ref="AC47" si="92">AB47</f>
         <v>60</v>
       </c>
     </row>
@@ -12580,7 +12580,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" ref="K53:K93" si="100">J53</f>
+        <f t="shared" ref="K53:K60" si="100">J53</f>
         <v>0</v>
       </c>
       <c r="L53" s="15">
@@ -12592,7 +12592,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="12">
-        <f t="shared" ref="O53:O93" si="101">N53</f>
+        <f t="shared" ref="O53:O60" si="101">N53</f>
         <v>0</v>
       </c>
       <c r="P53" s="15">
@@ -12607,7 +12607,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="12">
-        <f t="shared" ref="S53:S93" si="102">R53</f>
+        <f t="shared" ref="S53:S60" si="102">R53</f>
         <v>1</v>
       </c>
       <c r="T53" s="15">
@@ -12622,7 +12622,7 @@
         <v>1.2</v>
       </c>
       <c r="W53" s="12">
-        <f t="shared" ref="W53:W93" si="103">V53</f>
+        <f t="shared" ref="W53:W60" si="103">V53</f>
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
@@ -12637,7 +12637,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53" s="12">
-        <f t="shared" ref="AA53:AA93" si="104">Z53</f>
+        <f t="shared" ref="AA53:AA60" si="104">Z53</f>
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
@@ -13447,7 +13447,7 @@
         <v>9.6</v>
       </c>
       <c r="K62" s="40">
-        <f t="shared" ref="K62:K93" si="110">J62</f>
+        <f t="shared" ref="K62:K79" si="110">J62</f>
         <v>0</v>
       </c>
       <c r="L62" s="41">
@@ -13459,7 +13459,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="40">
-        <f t="shared" ref="O62:O93" si="111">N62</f>
+        <f t="shared" ref="O62:O79" si="111">N62</f>
         <v>0</v>
       </c>
       <c r="P62" s="41">
@@ -13474,7 +13474,7 @@
         <v>3.5</v>
       </c>
       <c r="S62" s="40">
-        <f t="shared" ref="S62:S93" si="112">R62</f>
+        <f t="shared" ref="S62:S79" si="112">R62</f>
         <v>3.5</v>
       </c>
       <c r="T62" s="41">
@@ -13489,7 +13489,7 @@
         <v>10</v>
       </c>
       <c r="W62" s="40">
-        <f t="shared" ref="W62:W93" si="113">V62</f>
+        <f t="shared" ref="W62:W79" si="113">V62</f>
         <v>10</v>
       </c>
       <c r="X62" s="41">
@@ -13504,7 +13504,7 @@
         <v>10</v>
       </c>
       <c r="AA62" s="40">
-        <f t="shared" ref="AA62:AA93" si="114">Z62</f>
+        <f t="shared" ref="AA62:AA79" si="114">Z62</f>
         <v>10</v>
       </c>
       <c r="AB62" s="41">

</xml_diff>